<commit_message>
Added Debugging and cleaned the code a bit
</commit_message>
<xml_diff>
--- a/tests/output_tests_data/transactions_output.xlsx
+++ b/tests/output_tests_data/transactions_output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="212">
   <si>
     <t>PharmBills System</t>
   </si>
@@ -34,544 +34,622 @@
     <t>Amount</t>
   </si>
   <si>
-    <t>5f968c36-ff56-40dd-8ef5-5db423316cfd</t>
+    <t>b5c423de-e76d-40b3-8393-618b4f612aee</t>
+  </si>
+  <si>
+    <t>10-02-2023</t>
   </si>
   <si>
     <t>Amerigroup</t>
   </si>
   <si>
-    <t>6d41f287-b597-4e05-8576-dab331d73fcc</t>
+    <t>fa325138-09d8-4371-85ec-c13ac78b1298</t>
+  </si>
+  <si>
+    <t>10-04-2023</t>
   </si>
   <si>
     <t>Preauthorized Credit</t>
   </si>
   <si>
-    <t>4bf660a8-9194-473e-ae1d-c643aa3c072e</t>
+    <t>3211f89b-d9c0-49fc-a692-3e94203e978a</t>
+  </si>
+  <si>
+    <t>10-23-2023</t>
   </si>
   <si>
     <t>uhc</t>
   </si>
   <si>
-    <t>dccc16a6-a8f6-4bff-abeb-25fa913e8f23</t>
-  </si>
-  <si>
-    <t>f52ace5a-2a4f-4cf9-957f-6379eb314569</t>
+    <t>524d08c6-33d1-4062-94c9-5d4bb2d6cedc</t>
+  </si>
+  <si>
+    <t>c400144c-0e4a-4f39-9b5c-aaedf357befe</t>
+  </si>
+  <si>
+    <t>10-11-2023</t>
   </si>
   <si>
     <t>Horizon NJ Health</t>
   </si>
   <si>
-    <t>c50e7f7c-755a-4b87-9860-e36502ace1a2</t>
-  </si>
-  <si>
-    <t>44b1f176-0db7-4f4e-938a-7e62b8c41858</t>
-  </si>
-  <si>
-    <t>561e138f-dea2-4201-a783-f47b50e4ed46</t>
-  </si>
-  <si>
-    <t>4a1e2904-425a-4a69-ad64-4a6c4b03acb9</t>
-  </si>
-  <si>
-    <t>968cf18d-16aa-4914-88e4-a357e822c460</t>
-  </si>
-  <si>
-    <t>30e21419-175f-4ce2-b2f3-065020f0009d</t>
-  </si>
-  <si>
-    <t>035c69dd-2a77-454b-8ca7-55f39f5d9f36</t>
-  </si>
-  <si>
-    <t>10e9d5b5-8d85-4caa-a11f-8a6a67b6b67d</t>
-  </si>
-  <si>
-    <t>e7203208-bec9-4ccc-9f47-819cc95badcb</t>
-  </si>
-  <si>
-    <t>7f7581c5-be27-4d1b-86a1-7f6c579b42a6</t>
-  </si>
-  <si>
-    <t>1720126a-d701-4f44-a67e-e3fc43465a30</t>
-  </si>
-  <si>
-    <t>9b78e464-3cc2-4c1f-b2e1-58ec91aa1cde</t>
+    <t>b658be36-d28c-4495-870c-55eca20e7986</t>
+  </si>
+  <si>
+    <t>66c2c6b9-8526-4da5-af66-da8d6110450c</t>
+  </si>
+  <si>
+    <t>10-05-2023</t>
+  </si>
+  <si>
+    <t>a71b50ab-3ca6-4264-b83e-1d0882ca9637</t>
+  </si>
+  <si>
+    <t>10-10-2023</t>
+  </si>
+  <si>
+    <t>fc2ecc76-b7bc-47ce-89bf-1af4a0d7fb8c</t>
+  </si>
+  <si>
+    <t>10-18-2023</t>
+  </si>
+  <si>
+    <t>d8997bd3-28f8-4986-8c38-804724b027b4</t>
+  </si>
+  <si>
+    <t>f00df1f9-7b24-4179-b3b5-a925bda748f7</t>
+  </si>
+  <si>
+    <t>10-25-2023</t>
+  </si>
+  <si>
+    <t>eb6d0635-20c1-420c-80d6-280c4f80619a</t>
+  </si>
+  <si>
+    <t>ca6ea29e-c497-4e07-ba02-e81d6ea9eb1d</t>
+  </si>
+  <si>
+    <t>10-13-2023</t>
+  </si>
+  <si>
+    <t>05555246-49df-4631-aeb7-fc519d65a930</t>
+  </si>
+  <si>
+    <t>10-17-2023</t>
+  </si>
+  <si>
+    <t>c1a4d16b-9a79-4e9d-9a88-661b5693b641</t>
+  </si>
+  <si>
+    <t>10-09-2023</t>
+  </si>
+  <si>
+    <t>5b800bff-4f87-4fd9-a88f-86bf52bb71c3</t>
+  </si>
+  <si>
+    <t>9ee05177-d353-40b0-8489-eeaaeacd10d0</t>
   </si>
   <si>
     <t>facility depost</t>
   </si>
   <si>
-    <t>5950ee78-0f33-44ce-87f1-6c477217324a</t>
+    <t>81a5664a-72db-4eb1-956c-b2f699f692dc</t>
   </si>
   <si>
     <t>Remote Deposit</t>
   </si>
   <si>
-    <t>413e2e83-6246-4041-807b-b6814f31a640</t>
-  </si>
-  <si>
-    <t>60f0baaa-0320-45d4-a0d9-50d050d72bfa</t>
-  </si>
-  <si>
-    <t>8b09a3da-f98b-422a-95b3-772bd6815119</t>
+    <t>af9442e5-d2ea-4fc8-a104-37697e0e0dc2</t>
+  </si>
+  <si>
+    <t>10-06-2023</t>
+  </si>
+  <si>
+    <t>078d6f79-8c69-410b-ba9f-1d1c0afabdb4</t>
+  </si>
+  <si>
+    <t>035ddaa5-fc9a-4c9e-8417-4b69c3575389</t>
   </si>
   <si>
     <t>rfms</t>
   </si>
   <si>
-    <t>9ce0918f-2aa2-4ed6-a102-69bf3fb09939</t>
-  </si>
-  <si>
-    <t>f37684ec-abd0-459b-afaf-16d314403452</t>
-  </si>
-  <si>
-    <t>9c28ccb8-57f6-43c8-8fdb-1a6bd4c23ff2</t>
-  </si>
-  <si>
-    <t>c13a3871-3b94-41dd-ac20-855598014141</t>
+    <t>30e85789-294f-41ac-a2d5-da36fca081aa</t>
+  </si>
+  <si>
+    <t>a3823378-cdbe-42e3-aee6-b9093356c5cc</t>
+  </si>
+  <si>
+    <t>7564ced3-f101-40ce-b0a6-9a45b0df4297</t>
+  </si>
+  <si>
+    <t>10-19-2023</t>
+  </si>
+  <si>
+    <t>9b8d13cb-7622-426d-aa51-014dc347fbb8</t>
   </si>
   <si>
     <t>facility deposit</t>
   </si>
   <si>
-    <t>2a9e1b3a-698e-4270-b052-733373607b12</t>
-  </si>
-  <si>
-    <t>3f2719be-deb5-43bc-bfef-90a584f5aa47</t>
+    <t>626c74f5-0a15-4ed9-9b61-d901ee3e67f5</t>
+  </si>
+  <si>
+    <t>de74ed21-5312-49ea-b438-ce76a62d28a1</t>
   </si>
   <si>
     <t>clover</t>
   </si>
   <si>
-    <t>129e0b89-7d72-45ce-b2a9-1b1533d06c34</t>
-  </si>
-  <si>
-    <t>486e758b-a4e6-4faa-8019-9490f472ad83</t>
+    <t>369f4523-a3d9-4e00-b430-5e733d2dbcfc</t>
+  </si>
+  <si>
+    <t>92340422-94e1-48ee-b669-f8059ff2b6c7</t>
   </si>
   <si>
     <t>fidelis</t>
   </si>
   <si>
-    <t>1c98af35-f3a3-4f64-bcb9-27ee3c62349c</t>
-  </si>
-  <si>
-    <t>8b9139a0-fffb-43ab-9aae-9776018a3f72</t>
-  </si>
-  <si>
-    <t>5e98ce70-d58e-4cfd-8136-ee412351c0a2</t>
-  </si>
-  <si>
-    <t>b6a22fa2-2764-4e63-8f0e-7335510a02b9</t>
-  </si>
-  <si>
-    <t>749ce875-0c6d-4bcf-a6f3-9dfd44c6da67</t>
-  </si>
-  <si>
-    <t>bebfc3d2-bc76-4642-a978-497e802ffbc8</t>
-  </si>
-  <si>
-    <t>51d5c2cb-caf0-4564-a719-ac16b4881c21</t>
-  </si>
-  <si>
-    <t>b835896f-3197-4ebd-8484-d406b5329523</t>
+    <t>77a6cdf8-9f07-4e15-b335-e072b0bf9bcb</t>
+  </si>
+  <si>
+    <t>1aa63f3d-2556-46be-9b4f-f0a5f76b6433</t>
+  </si>
+  <si>
+    <t>10-30-2023</t>
+  </si>
+  <si>
+    <t>99186afc-ffa0-49ab-bbd4-9d3c9b71f045</t>
+  </si>
+  <si>
+    <t>c4c4352f-b25e-431f-8704-39bc4fb78ff0</t>
+  </si>
+  <si>
+    <t>fa88baa4-8f5f-4950-879c-91b41e17c7d7</t>
+  </si>
+  <si>
+    <t>4212dce3-3fde-49d4-b01d-a2fc08400e0f</t>
+  </si>
+  <si>
+    <t>52ad48ff-cee8-448d-9faa-4f9307f3de14</t>
+  </si>
+  <si>
+    <t>ba1c853d-b7ba-4d00-b275-6b0428f3f3ab</t>
   </si>
   <si>
     <t>optum roster</t>
   </si>
   <si>
-    <t>daec2987-ae1e-474e-8383-8b6f9b1fc459</t>
-  </si>
-  <si>
-    <t>26205daf-34a4-426a-84be-ab64e28ad095</t>
-  </si>
-  <si>
-    <t>9715188c-23af-4209-9c74-e93ac7bdd426</t>
-  </si>
-  <si>
-    <t>837b154c-75ec-46cb-9c4c-c4d4898f86ab</t>
-  </si>
-  <si>
-    <t>353723ac-fda7-4a79-a977-d0ed26df358f</t>
-  </si>
-  <si>
-    <t>f121ab2f-eeb6-4ef4-ac02-19cbe011e3c2</t>
-  </si>
-  <si>
-    <t>b1c6b7e3-7d5a-4e00-8fff-4d037b7a11af</t>
-  </si>
-  <si>
-    <t>9688f7f7-2b58-44f0-b2f2-15460790c9f6</t>
-  </si>
-  <si>
-    <t>27448fac-56aa-43e9-853a-35aaa15d3018</t>
-  </si>
-  <si>
-    <t>2608b461-e942-4e25-aa02-fe2cba4d9f1c</t>
+    <t>86851b1b-bcc7-4801-876b-f24cd5647c35</t>
+  </si>
+  <si>
+    <t>c841c282-20a9-4994-b746-297c8777926f</t>
+  </si>
+  <si>
+    <t>012cfac8-7b53-4808-83f6-7076c40d3d31</t>
+  </si>
+  <si>
+    <t>479a5e1c-feaa-4174-b607-0186fa88d836</t>
+  </si>
+  <si>
+    <t>8a5ace14-90ae-4a13-a60b-76ad3db779e6</t>
+  </si>
+  <si>
+    <t>993ab4dc-794b-4b08-aa74-93463fa2e89e</t>
+  </si>
+  <si>
+    <t>810985e5-77cb-45dd-9466-5b030d90f280</t>
+  </si>
+  <si>
+    <t>a4d45f7f-a9bb-4d3c-99b7-12a5804734c7</t>
+  </si>
+  <si>
+    <t>73148938-de4f-4c5f-ba0e-87732a21b185</t>
+  </si>
+  <si>
+    <t>0ba03674-cb8e-4c83-b942-13ec5a918612</t>
   </si>
   <si>
     <t>Aetna Better Health</t>
   </si>
   <si>
-    <t>6723ac6e-8bb0-44c5-a636-b162c8d10952</t>
-  </si>
-  <si>
-    <t>2c3c9e33-1177-45a5-a104-e26e7c8cd26c</t>
-  </si>
-  <si>
-    <t>8a608c92-1d19-431b-bf34-3d43307f38ba</t>
-  </si>
-  <si>
-    <t>dadbba7b-90dc-4de0-8f42-0202926451e2</t>
-  </si>
-  <si>
-    <t>d1542409-60d0-49a0-8c7e-c1ffdfdfc82d</t>
-  </si>
-  <si>
-    <t>fdd2fcbb-1a69-456c-8b18-264df992d5f9</t>
-  </si>
-  <si>
-    <t>00a4da69-96e2-4f34-a2f8-8ff6262100d9</t>
-  </si>
-  <si>
-    <t>96a20c38-477c-4a86-a012-6df9475b1a7d</t>
-  </si>
-  <si>
-    <t>62efd51e-1d99-44aa-b1f0-265b72147a5c</t>
-  </si>
-  <si>
-    <t>949e1966-4c84-4b77-9fa1-607af5b8b3a5</t>
-  </si>
-  <si>
-    <t>89fef81d-7bca-4e98-9d2b-399692351724</t>
-  </si>
-  <si>
-    <t>d1f014fd-fa0b-44bc-bd13-8da9be2839cd</t>
-  </si>
-  <si>
-    <t>34c42810-2591-46df-89ae-479fd7b3c5d7</t>
-  </si>
-  <si>
-    <t>cb36f09a-b5b5-40ac-89a8-8665bfa9238a</t>
-  </si>
-  <si>
-    <t>d38c92f5-0f3b-4662-82d6-36a20d43cd90</t>
-  </si>
-  <si>
-    <t>5df5d9ec-4fd4-4c35-9623-64b7cc70aa99</t>
-  </si>
-  <si>
-    <t>f4a8671c-d667-4e75-a7b1-c6860696fd57</t>
-  </si>
-  <si>
-    <t>5a31a7c3-0763-4979-8f7b-fadf5da5b44f</t>
-  </si>
-  <si>
-    <t>5f8c3095-de57-435e-a16c-b9f8b557d8d5</t>
-  </si>
-  <si>
-    <t>e7bb51f7-1ae4-482a-b1fd-516279242ce8</t>
-  </si>
-  <si>
-    <t>4b1ed0d2-3a19-4f8f-91c3-768928860781</t>
-  </si>
-  <si>
-    <t>04198514-7d9d-4f91-8835-19be0a8d2f2d</t>
-  </si>
-  <si>
-    <t>b2e72bff-a5ec-4209-98d8-a745ad26e7d0</t>
-  </si>
-  <si>
-    <t>76145d16-f5cf-4ca2-9737-afaa85a5d5be</t>
-  </si>
-  <si>
-    <t>d890569e-dadf-4c7f-808e-05e60cdfaa96</t>
-  </si>
-  <si>
-    <t>dcc73913-af35-4590-aaa6-5aad37cbd381</t>
-  </si>
-  <si>
-    <t>f77ec341-3b93-4097-b438-3e22fd1d6620</t>
-  </si>
-  <si>
-    <t>911a6d6b-bb6d-446f-8ee8-f91db5384356</t>
-  </si>
-  <si>
-    <t>89add2db-6a57-4e0c-8898-8c6201709c7c</t>
-  </si>
-  <si>
-    <t>cad40c7d-04d4-4cba-98d1-9be7d713a541</t>
-  </si>
-  <si>
-    <t>c00155e9-c796-41a8-b1e3-870b0886ab10</t>
-  </si>
-  <si>
-    <t>2b3c7bb8-4fb3-4b19-95aa-e3d24b06b073</t>
+    <t>5918f319-3512-4970-b7a4-21fca0375206</t>
+  </si>
+  <si>
+    <t>b4a824dc-b73d-4334-9fd5-6f0858571ffd</t>
+  </si>
+  <si>
+    <t>80bc1273-ebca-45bb-b450-01df2c57649d</t>
+  </si>
+  <si>
+    <t>1f83c880-8988-4b2a-ac0e-6fed43d3e4ac</t>
+  </si>
+  <si>
+    <t>2fe295af-5401-4bcb-90da-4c559d2c0f03</t>
+  </si>
+  <si>
+    <t>a0f62f35-0b64-456d-8255-75dccf272fb2</t>
+  </si>
+  <si>
+    <t>fc89f536-dbca-45e1-8871-109d75a2c00a</t>
+  </si>
+  <si>
+    <t>310f5128-9871-484a-b064-502868f2ba3c</t>
+  </si>
+  <si>
+    <t>10-24-2023</t>
+  </si>
+  <si>
+    <t>1c4b9129-7fdc-4c9a-a621-b26b162e2cd2</t>
+  </si>
+  <si>
+    <t>e2008615-de97-4a49-9bb1-bdc28655e1b5</t>
+  </si>
+  <si>
+    <t>187f163d-1445-49cc-9bb9-b32467bff13b</t>
+  </si>
+  <si>
+    <t>a6a3dff5-4211-4392-9ed4-601f16ab2bd5</t>
+  </si>
+  <si>
+    <t>72bedc1e-a150-4678-b895-84fcce8de06b</t>
+  </si>
+  <si>
+    <t>10-16-2023</t>
+  </si>
+  <si>
+    <t>1232a073-f610-4b9c-aead-a61aa0fdc3db</t>
+  </si>
+  <si>
+    <t>10-12-2023</t>
+  </si>
+  <si>
+    <t>fdcd7cc5-1ae1-453d-bc3a-3881b3f62495</t>
+  </si>
+  <si>
+    <t>5c92b5fd-7eb7-438d-86b4-21c5d722fe2e</t>
+  </si>
+  <si>
+    <t>7f1d3e51-2911-4ac9-abf2-55609d043bc3</t>
+  </si>
+  <si>
+    <t>8cb2e455-0221-4aee-b331-bc72a358996e</t>
+  </si>
+  <si>
+    <t>c4a440bc-c0c2-4de9-bf04-e990fba0a882</t>
+  </si>
+  <si>
+    <t>e6142090-b0c9-43fc-833a-140b24aebf88</t>
+  </si>
+  <si>
+    <t>da2d95a6-83db-47eb-b92a-a7f1df995ee7</t>
+  </si>
+  <si>
+    <t>10-20-2023</t>
+  </si>
+  <si>
+    <t>a1479389-dce3-4abb-8c18-539a9a0df21e</t>
+  </si>
+  <si>
+    <t>674bc642-dbe8-4208-9414-986352d87b83</t>
+  </si>
+  <si>
+    <t>e749aad3-a182-49b2-b0e5-0b94517a6cfa</t>
+  </si>
+  <si>
+    <t>10-03-2023</t>
+  </si>
+  <si>
+    <t>47904d08-256f-4f38-8f58-f7cae68cf734</t>
+  </si>
+  <si>
+    <t>ca504ae7-b868-4d4b-b0cb-db1423187f7b</t>
+  </si>
+  <si>
+    <t>10-01-2023</t>
+  </si>
+  <si>
+    <t>39e84944-7e90-421a-b6c9-ff7f1b14b7d0</t>
+  </si>
+  <si>
+    <t>8bec7b40-488c-4646-9afe-8d6c05f91d2f</t>
+  </si>
+  <si>
+    <t>13457bfe-0af7-44e0-8499-a9181cf07288</t>
+  </si>
+  <si>
+    <t>9b6a3e3b-a7ca-4f45-9a83-2315e91319b8</t>
+  </si>
+  <si>
+    <t>1de0ffc3-da71-4951-8712-418e10511698</t>
+  </si>
+  <si>
+    <t>d00869fa-aefe-4819-9570-c18df06bd002</t>
   </si>
   <si>
     <t>credit card</t>
   </si>
   <si>
-    <t>af424cca-2c3a-4aa0-a6e4-476ef94c5dd8</t>
-  </si>
-  <si>
-    <t>4647ba47-c717-4715-889a-717f1a368f1a</t>
-  </si>
-  <si>
-    <t>d3a968e5-623a-4e5f-b6c6-c2f0ff83873c</t>
-  </si>
-  <si>
-    <t>05436dcd-c594-4f2d-8c61-baf22e766cc1</t>
-  </si>
-  <si>
-    <t>dce5b560-e12a-47de-8580-2e09edc8c9be</t>
-  </si>
-  <si>
-    <t>9d774c61-0eaf-414e-825a-0332e493cb07</t>
-  </si>
-  <si>
-    <t>62e8b055-baaf-484f-9b36-ddb11bd4836b</t>
-  </si>
-  <si>
-    <t>1e48b3ad-decd-46c6-9892-5cd920fb1108</t>
-  </si>
-  <si>
-    <t>216586a7-ccab-4b22-bc2e-5005703e866d</t>
-  </si>
-  <si>
-    <t>3b0b1928-48e5-4c3e-838a-93f95ee77967</t>
-  </si>
-  <si>
-    <t>577b3c8c-8f48-47b9-852a-1fbe77b31353</t>
-  </si>
-  <si>
-    <t>2f867050-f7f4-46e0-a25c-fd8d4b839bb3</t>
-  </si>
-  <si>
-    <t>4fb80e98-4d2e-42da-8fc8-89b8661c9d59</t>
-  </si>
-  <si>
-    <t>91c15905-47a1-48b1-a3b6-9e933e093031</t>
-  </si>
-  <si>
-    <t>0c8233a9-863d-4a79-b114-930ae36b7a44</t>
-  </si>
-  <si>
-    <t>e41697df-3d1a-43de-afab-4a62619b2193</t>
-  </si>
-  <si>
-    <t>80dfaceb-0f15-4ca1-af3c-c30f360e0300</t>
-  </si>
-  <si>
-    <t>e245c454-18d7-4fb4-a259-66606894d4c3</t>
-  </si>
-  <si>
-    <t>04e6b44c-641e-4c58-b49c-508f738f3628</t>
-  </si>
-  <si>
-    <t>1b73fcb9-eefb-4508-b417-467a01ca9aa0</t>
-  </si>
-  <si>
-    <t>cce132ac-7bfe-42d9-a3e2-088b22d6b86d</t>
-  </si>
-  <si>
-    <t>16109aa3-60e6-49b2-b45e-c4504c5fe35c</t>
-  </si>
-  <si>
-    <t>9c219576-4a39-4f6c-bc74-7283691eee9a</t>
-  </si>
-  <si>
-    <t>0cb6f17c-af3e-47d5-94e3-8d59c6430651</t>
-  </si>
-  <si>
-    <t>0bdeec34-0d4e-4abc-8c77-84474b4d65ab</t>
-  </si>
-  <si>
-    <t>f69415b8-4116-4684-a42f-50e09d0b98f4</t>
-  </si>
-  <si>
-    <t>29ef956c-2fea-478e-aae2-9345564abffc</t>
+    <t>ad40e202-2fec-419e-b3ab-742d232afeac</t>
+  </si>
+  <si>
+    <t>f581afeb-9e23-45a1-bb39-e4ad9c4394a0</t>
+  </si>
+  <si>
+    <t>10-26-2023</t>
+  </si>
+  <si>
+    <t>58748c93-1e7c-40fc-bc38-98319348b4f2</t>
+  </si>
+  <si>
+    <t>5d59ecb2-57d4-407b-a985-06520953bec4</t>
+  </si>
+  <si>
+    <t>ec32fa8c-398a-43d7-a900-f783633906b4</t>
+  </si>
+  <si>
+    <t>fc79a1f4-e157-429e-8805-f8e154a76679</t>
+  </si>
+  <si>
+    <t>c1233ff3-3bc5-4ad2-a578-860c085571fe</t>
+  </si>
+  <si>
+    <t>3b3598db-500f-44ba-98cf-0d3e7d60804c</t>
+  </si>
+  <si>
+    <t>10-08-2023</t>
+  </si>
+  <si>
+    <t>a727fee6-59d6-41d5-8497-f21ddb10c5f8</t>
+  </si>
+  <si>
+    <t>c0162977-4039-4a82-944e-f3e7039dae3a</t>
+  </si>
+  <si>
+    <t>ff649011-e41f-4a6a-b4c5-60122c70650c</t>
+  </si>
+  <si>
+    <t>434a2dc4-8822-45ba-b0a3-a24178bcc964</t>
+  </si>
+  <si>
+    <t>db65b99a-e2f7-49ee-b686-35112902421c</t>
+  </si>
+  <si>
+    <t>9ca76f52-013a-4e9a-b104-8cbe391c758b</t>
+  </si>
+  <si>
+    <t>10-31-2023</t>
+  </si>
+  <si>
+    <t>0f8cc650-a209-45ff-8bb3-617c7b175b49</t>
+  </si>
+  <si>
+    <t>19351df0-3ea0-4e95-8a5b-b1e3bf350b6b</t>
+  </si>
+  <si>
+    <t>181b12e4-75aa-4d12-a7b4-1d5c34388b6f</t>
+  </si>
+  <si>
+    <t>b63b6ffc-0f81-4955-be5b-dbf7f7a9d30d</t>
+  </si>
+  <si>
+    <t>eff7cf68-3568-48d3-a8e4-1cb1b2d5d974</t>
+  </si>
+  <si>
+    <t>ca2e10e5-f3bb-4eb1-97ed-f6c7ef3b6ab4</t>
+  </si>
+  <si>
+    <t>eae0870e-2704-4fd8-b7a2-98188e094485</t>
+  </si>
+  <si>
+    <t>4222a4e5-64f3-425b-8859-ec7df3e921e8</t>
+  </si>
+  <si>
+    <t>1169df88-b98c-45e8-aed4-96275515fae2</t>
+  </si>
+  <si>
+    <t>77d2324a-564c-451c-89dc-c795c79b35f4</t>
+  </si>
+  <si>
+    <t>ef6eaa2b-a7c6-4473-b4a0-ed36b3c0e255</t>
+  </si>
+  <si>
+    <t>4d96041b-9f82-4255-a31b-673fcae49f3c</t>
+  </si>
+  <si>
+    <t>3d4cd8fd-3018-41c2-8be8-67a9013f175f</t>
   </si>
   <si>
     <t>gnss wire 9/5/23</t>
   </si>
   <si>
-    <t>1526e407-1a74-48dc-acfb-2aebe36dad99</t>
-  </si>
-  <si>
-    <t>ab056eae-5b8b-4126-823d-2f62c2aa558e</t>
+    <t>6f086a51-bcf5-49db-80a2-584200266518</t>
+  </si>
+  <si>
+    <t>29c94398-7b65-415c-a863-75378b44ad5c</t>
   </si>
   <si>
     <t>wellmed cc</t>
   </si>
   <si>
-    <t>77b1bdc3-166b-466f-8441-3a280492559d</t>
+    <t>0888ab40-557e-4512-a658-b091c5187e14</t>
   </si>
   <si>
     <t>humana cc</t>
   </si>
   <si>
-    <t>d56072f4-3ccc-4739-b8b7-435e1f695297</t>
-  </si>
-  <si>
-    <t>476f7b72-9c06-45c9-a320-d6287f3aac73</t>
+    <t>6b190701-33ac-4ed1-b248-b72795ef335a</t>
+  </si>
+  <si>
+    <t>8ae3b5c6-32f7-4631-be20-d9499ac7ef54</t>
   </si>
   <si>
     <t>gnss wire back up</t>
   </si>
   <si>
-    <t>d4c5531f-df65-4cf1-8df8-63575932aa26</t>
+    <t>4e93fc18-18a7-4b3c-abed-2f90bed45f6e</t>
   </si>
   <si>
     <t>wire</t>
   </si>
   <si>
-    <t>37a49cfd-8b65-4059-a430-89e77585e47c</t>
+    <t>8a950839-6f95-4e7e-b7e5-88a7a9e18e8c</t>
   </si>
   <si>
     <t>gnss wire</t>
   </si>
   <si>
-    <t>5501343b-485a-4ffa-9f09-a643dc2862f2</t>
+    <t>911868da-700b-4e50-a346-71d12c42954e</t>
   </si>
   <si>
     <t>genesis wire 10/5/23</t>
   </si>
   <si>
-    <t>a4975ed1-2f72-4a4e-98dc-02d9595d178c</t>
-  </si>
-  <si>
-    <t>67185047-dcb7-4648-aec0-125306dececb</t>
-  </si>
-  <si>
-    <t>030fd7a9-b129-4728-a671-3ea288673c57</t>
+    <t>3f8872cc-7207-4607-b0d7-ced03cf5af2d</t>
+  </si>
+  <si>
+    <t>f2b6bff9-d2f2-4938-8e99-be48de31e638</t>
+  </si>
+  <si>
+    <t>1a328145-4fcc-46a7-9153-cd5a061c2e7a</t>
   </si>
   <si>
     <t>RFMS</t>
   </si>
   <si>
-    <t>d49f2edf-7025-4236-ae33-1bd513541110</t>
-  </si>
-  <si>
-    <t>62ff7e81-f5f8-4f90-9b5b-a16648e3b4c3</t>
-  </si>
-  <si>
-    <t>e3f70d7a-5664-44ec-8fde-6190257348e6</t>
-  </si>
-  <si>
-    <t>0f4d54de-fd9a-4f26-8cfb-368e5a0757e0</t>
-  </si>
-  <si>
-    <t>05439f76-aca6-4f49-a429-67c7031c5c6b</t>
-  </si>
-  <si>
-    <t>ec68e884-0d80-42d9-a9aa-254dac49f8b9</t>
-  </si>
-  <si>
-    <t>344d69bc-6654-4e9e-8b8d-41cc8f45db37</t>
-  </si>
-  <si>
-    <t>636b7544-7f8b-4453-8766-b998acaee934</t>
-  </si>
-  <si>
-    <t>9c66526f-e7af-4343-99b3-cddfb2b323f7</t>
-  </si>
-  <si>
-    <t>3d24543a-54e2-4b2d-8421-27b5632c9b35</t>
-  </si>
-  <si>
-    <t>2aa94b5e-7216-4d88-ac8d-6c7dacc8ece8</t>
+    <t>6973ded6-84e6-468f-9df6-9bdeccc8b361</t>
+  </si>
+  <si>
+    <t>11-01-2023</t>
+  </si>
+  <si>
+    <t>d7f26021-f35f-4aaa-a672-246be93db23b</t>
+  </si>
+  <si>
+    <t>11-02-2023</t>
+  </si>
+  <si>
+    <t>90888aac-b584-431c-9145-9e0749225471</t>
+  </si>
+  <si>
+    <t>2a9a50cd-0e88-4084-815d-79fdf83becf8</t>
+  </si>
+  <si>
+    <t>e061fdd6-16dc-4fc3-b71a-2348f64d8100</t>
+  </si>
+  <si>
+    <t>5a0ea32f-6ccd-48f8-9cac-638ffdad11b6</t>
+  </si>
+  <si>
+    <t>615de629-5dac-4b4f-85f2-57a1907e44d2</t>
+  </si>
+  <si>
+    <t>2d49192e-aa4e-42e6-8589-835e9e336ec6</t>
+  </si>
+  <si>
+    <t>e72fc340-499d-483e-a511-0328eeb848a5</t>
+  </si>
+  <si>
+    <t>abfc1344-ca55-4ebd-a87e-6fca7c20f842</t>
+  </si>
+  <si>
+    <t>81733169-a05d-4fb6-84e0-deacd5fa7cef</t>
   </si>
   <si>
     <t>hnjh ( total is 3681.72)</t>
   </si>
   <si>
-    <t>a5c2252c-693b-40ac-a6bd-0a3674344f67</t>
-  </si>
-  <si>
-    <t>b046fea9-84e8-4883-bd61-90fb459133f3</t>
-  </si>
-  <si>
-    <t>7a4a6d77-c791-4b8a-a6b9-a86fca2b782a</t>
-  </si>
-  <si>
-    <t>a5864da6-6d77-4a55-8880-79fa507c6b5f</t>
-  </si>
-  <si>
-    <t>c95e5d32-bd6f-4899-ba64-89731d3d8f84</t>
-  </si>
-  <si>
-    <t>ce4eeec3-2475-4f2f-ba26-65c9405db392</t>
-  </si>
-  <si>
-    <t>41f928bb-d8d2-4d0c-be1f-3fbf7d0959d3</t>
-  </si>
-  <si>
-    <t>6a99f4cc-aa9f-4387-9f19-f3ebf6932efb</t>
-  </si>
-  <si>
-    <t>293333b4-81df-4052-bf4a-a02b1b908243</t>
-  </si>
-  <si>
-    <t>aae6d74b-3f81-44ec-8cf8-723a84d3014a</t>
-  </si>
-  <si>
-    <t>c8473900-cb3a-4eaa-9aec-42997f2595f1</t>
+    <t>483ecf4e-acaf-44f4-89ec-713be8948233</t>
+  </si>
+  <si>
+    <t>adcf3d2a-6e39-403d-8168-dac5f4a28453</t>
+  </si>
+  <si>
+    <t>64fb5501-54b6-490f-ab38-318ae469e0c4</t>
+  </si>
+  <si>
+    <t>5bef6648-1fc4-46c3-a5e6-56a7da6b47c6</t>
+  </si>
+  <si>
+    <t>8a79e555-b7ae-421c-b842-1669a18a6b8f</t>
+  </si>
+  <si>
+    <t>ce90d9c4-49d9-4c2f-bd39-93485198cbd8</t>
+  </si>
+  <si>
+    <t>4b650895-17b8-4797-a7ce-813ee50053cb</t>
+  </si>
+  <si>
+    <t>f0b03a16-2bda-4294-94a0-d5629248899a</t>
+  </si>
+  <si>
+    <t>25fb0bde-b48e-4323-bef5-36b50aba3d5c</t>
+  </si>
+  <si>
+    <t>68eeb0e7-d091-4975-93fe-a167402783b7</t>
+  </si>
+  <si>
+    <t>8d5ba629-f416-498d-a5cd-d739d782de05</t>
   </si>
   <si>
     <t>gen wire</t>
   </si>
   <si>
-    <t>5326dc25-f514-46b6-b0fd-e69d647c8a89</t>
+    <t>3530226c-de7a-46fd-a488-edb7785f44e8</t>
   </si>
   <si>
     <t>uhc cc</t>
   </si>
   <si>
-    <t>18539994-fe8a-4264-862a-1eb2f566206a</t>
-  </si>
-  <si>
-    <t>6e586d92-f057-4ff7-b448-82171c3eed24</t>
+    <t>253866b6-caca-4de9-a3a8-a1c783f8caf2</t>
+  </si>
+  <si>
+    <t>2fa824da-ae1e-449e-883a-2e28daac9675</t>
+  </si>
+  <si>
+    <t>10-27-2023</t>
   </si>
   <si>
     <t>Automatic Transfer</t>
   </si>
   <si>
-    <t>372b5a60-bd3e-4951-92b9-e2d1ba220a19</t>
-  </si>
-  <si>
-    <t>150ca95c-60ce-443f-8624-b019a0a5185b</t>
-  </si>
-  <si>
-    <t>2cabd4f8-f201-4dc5-88bd-8de570b3eae0</t>
-  </si>
-  <si>
-    <t>aab15687-833b-4a56-b719-5c5a9e778856</t>
-  </si>
-  <si>
-    <t>58d650ea-a912-41fd-9420-f2c1471eeb1c</t>
-  </si>
-  <si>
-    <t>e0cd5dbc-a0c0-4352-83e8-21bbcf8638f4</t>
-  </si>
-  <si>
-    <t>870ae392-762e-4a06-b697-839a423e582d</t>
-  </si>
-  <si>
-    <t>d64fe4a7-cb45-4912-903a-fccfd03ce8c3</t>
-  </si>
-  <si>
-    <t>82b63c47-4d15-4e1f-af45-8bee6db5380e</t>
-  </si>
-  <si>
-    <t>f64dbeeb-7e8a-4cef-bd0d-c5e49484a250</t>
-  </si>
-  <si>
-    <t>51c30b2d-69ac-4d9d-b821-5cb41860e178</t>
-  </si>
-  <si>
-    <t>a9873f8e-d194-4d07-8cbb-dcc9af18cfa1</t>
-  </si>
-  <si>
-    <t>bdec70f0-652d-4e1b-ac33-f4155c48da9a</t>
+    <t>64d25d73-7e2a-4682-9891-36132a2e6dd5</t>
+  </si>
+  <si>
+    <t>ea3db43b-0ce2-48ac-b50d-3bb298f47368</t>
+  </si>
+  <si>
+    <t>b9c5c832-c796-43db-8bc0-eba636b52e01</t>
+  </si>
+  <si>
+    <t>deb88a2c-58ad-4506-a5fc-d00a78c153ee</t>
+  </si>
+  <si>
+    <t>4764da6c-db6c-4c98-a2c2-d9dc1ff554b4</t>
+  </si>
+  <si>
+    <t>d0d9920c-bb9f-4d3a-a4d9-e439b65c80ce</t>
+  </si>
+  <si>
+    <t>5c6cb285-fb98-4fad-9b85-1802f32315d0</t>
+  </si>
+  <si>
+    <t>34d3e779-0c99-4b24-8aac-8e8d5ea551ca</t>
+  </si>
+  <si>
+    <t>760a8333-e853-4589-8da5-d5ca6b24941c</t>
+  </si>
+  <si>
+    <t>21c4db43-c621-430e-83b3-ef5e55d6436c</t>
+  </si>
+  <si>
+    <t>c5b427fe-bd09-4865-99b8-73e3adfcad97</t>
+  </si>
+  <si>
+    <t>1d5e54ca-4288-4403-955a-0e88536d6c0d</t>
+  </si>
+  <si>
+    <t>a697d878-b0ac-4e7e-85ac-1e779ec6df22</t>
   </si>
 </sst>
 </file>
@@ -616,13 +694,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC0C0C0"/>
+        <fgColor rgb="FFFFC0CB"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFA8072"/>
+        <fgColor rgb="FFFF00FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1002,23 +1080,23 @@
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3">
-        <v>45201</v>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" s="3">
         <v>1794.93</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="3">
-        <v>45203</v>
+        <v>9</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I4" s="3">
         <v>1794.93</v>
@@ -1026,25 +1104,25 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="3">
-        <v>45222</v>
+        <v>12</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D5" s="3">
         <v>10</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="3">
-        <v>45222</v>
+        <v>15</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I5" s="3">
         <v>10</v>
@@ -1052,25 +1130,25 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="3">
-        <v>45210</v>
+        <v>16</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D6" s="3">
         <v>10892.88</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="3">
-        <v>45210</v>
+        <v>19</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I6" s="3">
         <v>10892.88</v>
@@ -1078,25 +1156,25 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="3">
-        <v>45204</v>
+        <v>20</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D7" s="3">
         <v>14605.06</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="3">
-        <v>45209</v>
+        <v>22</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I7" s="3">
         <v>14605.06</v>
@@ -1104,25 +1182,25 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="3">
-        <v>45217</v>
+        <v>24</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D8" s="3">
         <v>3600</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="3">
-        <v>45217</v>
+        <v>26</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I8" s="3">
         <v>3600</v>
@@ -1130,25 +1208,25 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="3">
-        <v>45224</v>
+        <v>27</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D9" s="3">
         <v>7442.7</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="3">
-        <v>45224</v>
+        <v>29</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I9" s="3">
         <v>7442.7</v>
@@ -1156,25 +1234,25 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="3">
-        <v>45212</v>
+        <v>30</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D10" s="3">
         <v>5276.55</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" s="3">
-        <v>45216</v>
+        <v>32</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I10" s="3">
         <v>5276.55</v>
@@ -1182,25 +1260,25 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="3">
-        <v>45208</v>
+        <v>34</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D11" s="3">
         <v>7967.17</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="3">
-        <v>45210</v>
+        <v>36</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I11" s="3">
         <v>7967.17</v>
@@ -1208,25 +1286,25 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="3">
-        <v>45216</v>
+        <v>37</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="D12" s="3">
         <v>19359.39</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G12" s="3">
-        <v>45216</v>
+        <v>39</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="I12" s="3">
         <v>19359.39</v>
@@ -1234,25 +1312,25 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="3">
-        <v>45205</v>
+        <v>41</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D13" s="3">
         <v>7600</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G13" s="3">
-        <v>45205</v>
+        <v>43</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I13" s="3">
         <v>7600</v>
@@ -1260,25 +1338,25 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="3">
-        <v>45203</v>
+        <v>44</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D14" s="3">
         <v>4273.85</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G14" s="3">
-        <v>45204</v>
+        <v>46</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I14" s="3">
         <v>4273.85</v>
@@ -1286,25 +1364,25 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="3">
-        <v>45216</v>
+        <v>47</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D15" s="3">
         <v>14003.8</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G15" s="3">
-        <v>45218</v>
+        <v>48</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I15" s="3">
         <v>14003.8</v>
@@ -1312,25 +1390,25 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="3">
-        <v>45205</v>
+        <v>50</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="D16" s="3">
         <v>13108.16</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G16" s="3">
-        <v>45205</v>
+        <v>52</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="I16" s="3">
         <v>13108.16</v>
@@ -1338,25 +1416,25 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="3">
-        <v>45201</v>
+        <v>53</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="D17" s="3">
         <v>3766</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G17" s="3">
-        <v>45201</v>
+        <v>55</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I17" s="3">
         <v>3766</v>
@@ -1364,25 +1442,25 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="3">
-        <v>45204</v>
+        <v>56</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="D18" s="3">
         <v>8118.05</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G18" s="3">
-        <v>45204</v>
+        <v>58</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I18" s="3">
         <v>8118.05</v>
@@ -1390,25 +1468,25 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" s="3">
-        <v>45229</v>
+        <v>59</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D19" s="3">
         <v>3894.87</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G19" s="3">
-        <v>45229</v>
+        <v>61</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I19" s="3">
         <v>3894.87</v>
@@ -1416,25 +1494,25 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20" s="3">
-        <v>45204</v>
+        <v>62</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D20" s="3">
         <v>24762.74</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G20" s="3">
-        <v>45204</v>
+        <v>63</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I20" s="3">
         <v>24762.74</v>
@@ -1442,25 +1520,25 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="3">
-        <v>45216</v>
+        <v>64</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D21" s="3">
         <v>66362.89999999999</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G21" s="3">
-        <v>45216</v>
+        <v>65</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I21" s="3">
         <v>66362.89999999999</v>
@@ -1468,25 +1546,25 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" s="3">
-        <v>45216</v>
+        <v>66</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="D22" s="3">
         <v>24000</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G22" s="3">
-        <v>45218</v>
+        <v>68</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I22" s="3">
         <v>24000</v>
@@ -1494,25 +1572,25 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B23" s="3">
-        <v>45210</v>
+        <v>69</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D23" s="3">
         <v>3525.52</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G23" s="3">
-        <v>45210</v>
+        <v>70</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I23" s="3">
         <v>3525.52</v>
@@ -1520,25 +1598,25 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B24" s="3">
-        <v>45229</v>
+        <v>71</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D24" s="3">
         <v>5191.8</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G24" s="3">
-        <v>45229</v>
+        <v>72</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I24" s="3">
         <v>5191.8</v>
@@ -1546,25 +1624,25 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B25" s="3">
-        <v>45210</v>
+        <v>73</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="D25" s="3">
         <v>36042.72</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G25" s="3">
-        <v>45210</v>
+        <v>74</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="I25" s="3">
         <v>36042.72</v>
@@ -1572,25 +1650,25 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B26" s="3">
-        <v>45212</v>
+        <v>75</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D26" s="3">
         <v>139340.44</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G26" s="3">
-        <v>45212</v>
+        <v>76</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I26" s="3">
         <v>139340.44</v>
@@ -1598,25 +1676,25 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B27" s="3">
-        <v>45210</v>
+        <v>77</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="D27" s="3">
         <v>31565.3</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G27" s="3">
-        <v>45210</v>
+        <v>79</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I27" s="3">
         <v>31565.3</v>
@@ -1624,25 +1702,25 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B28" s="3">
-        <v>45209</v>
+        <v>80</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="D28" s="3">
         <v>11854.8</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G28" s="3">
-        <v>45209</v>
+        <v>81</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I28" s="3">
         <v>11854.8</v>
@@ -1650,25 +1728,25 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B29" s="3">
-        <v>45203</v>
+        <v>82</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D29" s="3">
         <v>8400</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G29" s="3">
-        <v>45203</v>
+        <v>83</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I29" s="3">
         <v>8400</v>
@@ -1676,25 +1754,25 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B30" s="3">
-        <v>45217</v>
+        <v>84</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D30" s="3">
         <v>83152.14999999999</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G30" s="3">
-        <v>45217</v>
+        <v>85</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I30" s="3">
         <v>83152.14999999999</v>
@@ -1702,25 +1780,25 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B31" s="3">
-        <v>45223</v>
+        <v>86</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="D31" s="3">
         <v>57552.58</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G31" s="3">
-        <v>45223</v>
+        <v>88</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="I31" s="3">
         <v>57552.58</v>
@@ -1728,25 +1806,25 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B32" s="3">
-        <v>45218</v>
+        <v>89</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D32" s="3">
         <v>339.27</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G32" s="3">
-        <v>45222</v>
+        <v>90</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I32" s="3">
         <v>339.27</v>
@@ -1754,25 +1832,25 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B33" s="3">
-        <v>45212</v>
+        <v>91</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="D33" s="3">
         <v>212.1</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G33" s="3">
-        <v>45215</v>
+        <v>92</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I33" s="3">
         <v>212.1</v>
@@ -1780,25 +1858,25 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B34" s="3">
-        <v>45211</v>
+        <v>94</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="D34" s="3">
         <v>26453.7</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="G34" s="3">
-        <v>45210</v>
+        <v>96</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I34" s="3">
         <v>26453.7</v>
@@ -1806,25 +1884,25 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B35" s="3">
-        <v>45211</v>
+        <v>97</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="D35" s="3">
         <v>2646.4</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="G35" s="3">
-        <v>45211</v>
+        <v>98</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="I35" s="3">
         <v>2646.4</v>
@@ -1832,25 +1910,25 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B36" s="3">
-        <v>45215</v>
+        <v>99</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="D36" s="3">
         <v>24537.16</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="G36" s="3">
-        <v>45215</v>
+        <v>100</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I36" s="3">
         <v>24537.16</v>
@@ -1858,25 +1936,25 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B37" s="3">
-        <v>45218</v>
+        <v>101</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D37" s="3">
         <v>1753.23</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="G37" s="3">
-        <v>45219</v>
+        <v>102</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I37" s="3">
         <v>1753.23</v>
@@ -1884,25 +1962,25 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B38" s="3">
-        <v>45216</v>
+        <v>104</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D38" s="3">
         <v>219.17</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G38" s="3">
-        <v>45216</v>
+        <v>105</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I38" s="3">
         <v>219.17</v>
@@ -1910,25 +1988,25 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B39" s="3">
-        <v>45202</v>
+        <v>106</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D39" s="3">
         <v>63582.2</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="G39" s="3">
-        <v>45203</v>
+        <v>108</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I39" s="3">
         <v>63582.2</v>
@@ -1936,25 +2014,25 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B40" s="3">
-        <v>45200</v>
+        <v>109</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D40" s="3">
         <v>350.7</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="G40" s="3">
-        <v>45201</v>
+        <v>111</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I40" s="3">
         <v>350.7</v>
@@ -1962,25 +2040,25 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B41" s="3">
-        <v>45222</v>
+        <v>112</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D41" s="3">
         <v>35295.32</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="G41" s="3">
-        <v>45224</v>
+        <v>113</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I41" s="3">
         <v>35295.32</v>
@@ -1988,25 +2066,25 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B42" s="3">
-        <v>45203</v>
+        <v>114</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D42" s="3">
         <v>8931.24</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="G42" s="3">
-        <v>45203</v>
+        <v>115</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I42" s="3">
         <v>8931.24</v>
@@ -2014,25 +2092,25 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B43" s="3">
-        <v>45217</v>
+        <v>116</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="D43" s="3">
         <v>1764</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="G43" s="3">
-        <v>45218</v>
+        <v>118</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I43" s="3">
         <v>1764</v>
@@ -2040,25 +2118,25 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B44" s="3">
-        <v>45225</v>
+        <v>119</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D44" s="3">
         <v>8160</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="G44" s="3">
-        <v>45225</v>
+        <v>121</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I44" s="3">
         <v>8160</v>
@@ -2066,25 +2144,25 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B45" s="3">
-        <v>45217</v>
+        <v>122</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="D45" s="3">
         <v>7654.8</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="G45" s="3">
-        <v>45217</v>
+        <v>123</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I45" s="3">
         <v>7654.8</v>
@@ -2092,25 +2170,25 @@
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B46" s="3">
-        <v>45209</v>
+        <v>124</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D46" s="3">
         <v>10600</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="G46" s="3">
-        <v>45209</v>
+        <v>125</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I46" s="3">
         <v>10600</v>
@@ -2118,25 +2196,25 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B47" s="3">
-        <v>45207</v>
+        <v>126</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>127</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="D47" s="3">
         <v>6634.16</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="G47" s="3">
-        <v>45209</v>
+        <v>128</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I47" s="3">
         <v>6634.16</v>
@@ -2144,25 +2222,25 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B48" s="3">
-        <v>45224</v>
+        <v>129</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D48" s="3">
         <v>5226.3</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="G48" s="3">
-        <v>45224</v>
+        <v>130</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I48" s="3">
         <v>5226.3</v>
@@ -2170,25 +2248,25 @@
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B49" s="3">
-        <v>45200</v>
+        <v>131</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="D49" s="3">
         <v>1900</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="G49" s="3">
-        <v>45216</v>
+        <v>132</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I49" s="3">
         <v>1900</v>
@@ -2196,25 +2274,25 @@
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="B50" s="3">
-        <v>45230</v>
+        <v>133</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D50" s="3">
         <v>14700</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="G50" s="3">
-        <v>45230</v>
+        <v>135</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I50" s="3">
         <v>14700</v>
@@ -2222,25 +2300,25 @@
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B51" s="3">
-        <v>45216</v>
+        <v>136</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="D51" s="3">
         <v>16246.77</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="G51" s="3">
-        <v>45216</v>
+        <v>137</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="I51" s="3">
         <v>16246.77</v>
@@ -2248,25 +2326,25 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B52" s="3">
-        <v>45230</v>
+        <v>138</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D52" s="3">
         <v>6010.8</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="G52" s="3">
-        <v>45230</v>
+        <v>139</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I52" s="3">
         <v>6010.8</v>
@@ -2274,25 +2352,25 @@
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B53" s="3">
-        <v>45215</v>
+        <v>140</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D53" s="3">
         <v>127.26</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="G53" s="3">
-        <v>45215</v>
+        <v>141</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I53" s="3">
         <v>127.26</v>
@@ -2300,25 +2378,25 @@
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B54" s="4">
-        <v>45200</v>
+        <v>143</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>110</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="D54" s="4">
         <v>4784.89</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="G54" s="4">
-        <v>45201</v>
+        <v>142</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I54" s="4">
         <v>13684.89</v>
@@ -2326,25 +2404,25 @@
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="B55" s="4">
-        <v>45230</v>
+        <v>144</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>134</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D55" s="4">
         <v>250</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="G55" s="5">
-        <v>45211</v>
+        <v>149</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>95</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I55" s="5">
         <v>12315.5</v>
@@ -2352,25 +2430,25 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B56" s="4">
-        <v>45218</v>
+        <v>145</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="D56" s="4">
         <v>1800</v>
       </c>
       <c r="F56" t="s">
-        <v>170</v>
-      </c>
-      <c r="G56">
-        <v>45219</v>
+        <v>195</v>
+      </c>
+      <c r="G56" t="s">
+        <v>103</v>
       </c>
       <c r="H56" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I56">
         <v>16393.61</v>
@@ -2378,25 +2456,25 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="B57" s="4">
-        <v>45223</v>
+        <v>146</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="D57" s="4">
         <v>1850</v>
       </c>
       <c r="F57" t="s">
-        <v>171</v>
-      </c>
-      <c r="G57">
-        <v>45226</v>
+        <v>196</v>
+      </c>
+      <c r="G57" t="s">
+        <v>197</v>
       </c>
       <c r="H57" t="s">
-        <v>172</v>
+        <v>198</v>
       </c>
       <c r="I57">
         <v>8208.860000000001</v>
@@ -2404,25 +2482,25 @@
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="B58" s="4">
-        <v>45200</v>
+        <v>147</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>110</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="D58" s="4">
         <v>5000</v>
       </c>
       <c r="F58" t="s">
-        <v>173</v>
-      </c>
-      <c r="G58">
-        <v>45230</v>
+        <v>199</v>
+      </c>
+      <c r="G58" t="s">
+        <v>134</v>
       </c>
       <c r="H58" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="I58">
         <v>21264.4</v>
@@ -2430,25 +2508,25 @@
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="B59" s="5">
-        <v>45210</v>
+        <v>150</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
       <c r="D59" s="5">
         <v>7815.5</v>
       </c>
       <c r="F59" t="s">
-        <v>174</v>
-      </c>
-      <c r="G59">
-        <v>45212</v>
+        <v>200</v>
+      </c>
+      <c r="G59" t="s">
+        <v>31</v>
       </c>
       <c r="H59" t="s">
-        <v>172</v>
+        <v>198</v>
       </c>
       <c r="I59">
         <v>12315.96</v>
@@ -2456,25 +2534,25 @@
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="B60" s="5">
-        <v>45210</v>
+        <v>152</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>130</v>
+        <v>153</v>
       </c>
       <c r="D60" s="5">
         <v>3750</v>
       </c>
       <c r="F60" t="s">
-        <v>175</v>
-      </c>
-      <c r="G60">
-        <v>45225</v>
+        <v>201</v>
+      </c>
+      <c r="G60" t="s">
+        <v>120</v>
       </c>
       <c r="H60" t="s">
-        <v>172</v>
+        <v>198</v>
       </c>
       <c r="I60">
         <v>66343.42</v>
@@ -2482,25 +2560,25 @@
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="B61" s="5">
-        <v>45210</v>
+        <v>154</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>130</v>
+        <v>153</v>
       </c>
       <c r="D61" s="5">
         <v>750</v>
       </c>
       <c r="F61" t="s">
-        <v>176</v>
-      </c>
-      <c r="G61">
-        <v>45225</v>
+        <v>202</v>
+      </c>
+      <c r="G61" t="s">
+        <v>120</v>
       </c>
       <c r="H61" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I61">
         <v>1858.99</v>
@@ -2508,25 +2586,25 @@
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>132</v>
-      </c>
-      <c r="B62">
-        <v>45200</v>
+        <v>155</v>
+      </c>
+      <c r="B62" t="s">
+        <v>110</v>
       </c>
       <c r="C62" t="s">
-        <v>133</v>
+        <v>156</v>
       </c>
       <c r="D62">
         <v>0</v>
       </c>
       <c r="F62" t="s">
-        <v>177</v>
-      </c>
-      <c r="G62">
-        <v>45219</v>
+        <v>203</v>
+      </c>
+      <c r="G62" t="s">
+        <v>103</v>
       </c>
       <c r="H62" t="s">
-        <v>172</v>
+        <v>198</v>
       </c>
       <c r="I62">
         <v>17738.6</v>
@@ -2534,25 +2612,25 @@
     </row>
     <row r="63" spans="1:9">
       <c r="A63" t="s">
-        <v>134</v>
-      </c>
-      <c r="B63">
-        <v>45200</v>
+        <v>157</v>
+      </c>
+      <c r="B63" t="s">
+        <v>110</v>
       </c>
       <c r="C63" t="s">
-        <v>135</v>
+        <v>158</v>
       </c>
       <c r="D63">
         <v>6.72</v>
       </c>
       <c r="F63" t="s">
-        <v>178</v>
-      </c>
-      <c r="G63">
-        <v>45223</v>
+        <v>204</v>
+      </c>
+      <c r="G63" t="s">
+        <v>87</v>
       </c>
       <c r="H63" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I63">
         <v>5583.29</v>
@@ -2560,25 +2638,25 @@
     </row>
     <row r="64" spans="1:9">
       <c r="A64" t="s">
-        <v>136</v>
-      </c>
-      <c r="B64">
-        <v>45200</v>
+        <v>159</v>
+      </c>
+      <c r="B64" t="s">
+        <v>110</v>
       </c>
       <c r="C64" t="s">
-        <v>137</v>
+        <v>160</v>
       </c>
       <c r="D64">
         <v>5640.5</v>
       </c>
       <c r="F64" t="s">
-        <v>179</v>
-      </c>
-      <c r="G64">
-        <v>45222</v>
+        <v>205</v>
+      </c>
+      <c r="G64" t="s">
+        <v>13</v>
       </c>
       <c r="H64" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I64">
         <v>9694.860000000001</v>
@@ -2586,25 +2664,25 @@
     </row>
     <row r="65" spans="1:9">
       <c r="A65" t="s">
-        <v>138</v>
-      </c>
-      <c r="B65">
-        <v>45204</v>
+        <v>161</v>
+      </c>
+      <c r="B65" t="s">
+        <v>21</v>
       </c>
       <c r="C65" t="s">
-        <v>139</v>
+        <v>162</v>
       </c>
       <c r="D65">
         <v>7185</v>
       </c>
       <c r="F65" t="s">
-        <v>180</v>
-      </c>
-      <c r="G65">
-        <v>45203</v>
+        <v>206</v>
+      </c>
+      <c r="G65" t="s">
+        <v>10</v>
       </c>
       <c r="H65" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I65">
         <v>3681.72</v>
@@ -2612,25 +2690,25 @@
     </row>
     <row r="66" spans="1:9">
       <c r="A66" t="s">
-        <v>140</v>
-      </c>
-      <c r="B66">
-        <v>45230</v>
+        <v>163</v>
+      </c>
+      <c r="B66" t="s">
+        <v>134</v>
       </c>
       <c r="C66" t="s">
-        <v>130</v>
+        <v>153</v>
       </c>
       <c r="D66">
         <v>68.45999999999999</v>
       </c>
       <c r="F66" t="s">
-        <v>181</v>
-      </c>
-      <c r="G66">
-        <v>45226</v>
+        <v>207</v>
+      </c>
+      <c r="G66" t="s">
+        <v>197</v>
       </c>
       <c r="H66" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I66">
         <v>4335</v>
@@ -2638,25 +2716,25 @@
     </row>
     <row r="67" spans="1:9">
       <c r="A67" t="s">
-        <v>141</v>
-      </c>
-      <c r="B67">
-        <v>45200</v>
+        <v>164</v>
+      </c>
+      <c r="B67" t="s">
+        <v>110</v>
       </c>
       <c r="C67" t="s">
-        <v>137</v>
+        <v>160</v>
       </c>
       <c r="D67">
         <v>583.5</v>
       </c>
       <c r="F67" t="s">
-        <v>182</v>
-      </c>
-      <c r="G67">
-        <v>45202</v>
+        <v>208</v>
+      </c>
+      <c r="G67" t="s">
+        <v>107</v>
       </c>
       <c r="H67" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I67">
         <v>2805.74</v>
@@ -2664,25 +2742,25 @@
     </row>
     <row r="68" spans="1:9">
       <c r="A68" t="s">
-        <v>142</v>
-      </c>
-      <c r="B68">
-        <v>45230</v>
+        <v>165</v>
+      </c>
+      <c r="B68" t="s">
+        <v>134</v>
       </c>
       <c r="C68" t="s">
-        <v>143</v>
+        <v>166</v>
       </c>
       <c r="D68">
         <v>72.70999999999999</v>
       </c>
       <c r="F68" t="s">
-        <v>183</v>
-      </c>
-      <c r="G68">
-        <v>45210</v>
+        <v>209</v>
+      </c>
+      <c r="G68" t="s">
+        <v>17</v>
       </c>
       <c r="H68" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I68">
         <v>38264.2</v>
@@ -2690,25 +2768,25 @@
     </row>
     <row r="69" spans="1:9">
       <c r="A69" t="s">
-        <v>144</v>
-      </c>
-      <c r="B69">
-        <v>45231</v>
+        <v>167</v>
+      </c>
+      <c r="B69" t="s">
+        <v>168</v>
       </c>
       <c r="C69" t="s">
-        <v>143</v>
+        <v>166</v>
       </c>
       <c r="D69">
         <v>2179.23</v>
       </c>
       <c r="F69" t="s">
-        <v>184</v>
-      </c>
-      <c r="G69">
-        <v>45230</v>
+        <v>210</v>
+      </c>
+      <c r="G69" t="s">
+        <v>134</v>
       </c>
       <c r="H69" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I69">
         <v>505.02</v>
@@ -2716,25 +2794,25 @@
     </row>
     <row r="70" spans="1:9">
       <c r="A70" t="s">
-        <v>145</v>
-      </c>
-      <c r="B70">
-        <v>45232</v>
+        <v>169</v>
+      </c>
+      <c r="B70" t="s">
+        <v>170</v>
       </c>
       <c r="C70" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="D70">
         <v>1707</v>
       </c>
       <c r="F70" t="s">
-        <v>185</v>
-      </c>
-      <c r="G70">
-        <v>45224</v>
+        <v>211</v>
+      </c>
+      <c r="G70" t="s">
+        <v>28</v>
       </c>
       <c r="H70" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I70">
         <v>4604.06</v>
@@ -2742,13 +2820,13 @@
     </row>
     <row r="71" spans="1:9">
       <c r="A71" t="s">
-        <v>146</v>
-      </c>
-      <c r="B71">
-        <v>45222</v>
+        <v>171</v>
+      </c>
+      <c r="B71" t="s">
+        <v>13</v>
       </c>
       <c r="C71" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D71">
         <v>173.99</v>
@@ -2756,13 +2834,13 @@
     </row>
     <row r="72" spans="1:9">
       <c r="A72" t="s">
-        <v>147</v>
-      </c>
-      <c r="B72">
-        <v>45200</v>
+        <v>172</v>
+      </c>
+      <c r="B72" t="s">
+        <v>110</v>
       </c>
       <c r="C72" t="s">
-        <v>137</v>
+        <v>160</v>
       </c>
       <c r="D72">
         <v>703.4299999999999</v>
@@ -2770,13 +2848,13 @@
     </row>
     <row r="73" spans="1:9">
       <c r="A73" t="s">
-        <v>148</v>
-      </c>
-      <c r="B73">
-        <v>45223</v>
+        <v>173</v>
+      </c>
+      <c r="B73" t="s">
+        <v>87</v>
       </c>
       <c r="C73" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="D73">
         <v>2754.06</v>
@@ -2784,13 +2862,13 @@
     </row>
     <row r="74" spans="1:9">
       <c r="A74" t="s">
-        <v>149</v>
-      </c>
-      <c r="B74">
-        <v>45209</v>
+        <v>174</v>
+      </c>
+      <c r="B74" t="s">
+        <v>23</v>
       </c>
       <c r="C74" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D74">
         <v>14539</v>
@@ -2798,13 +2876,13 @@
     </row>
     <row r="75" spans="1:9">
       <c r="A75" t="s">
-        <v>150</v>
-      </c>
-      <c r="B75">
-        <v>45200</v>
+        <v>175</v>
+      </c>
+      <c r="B75" t="s">
+        <v>110</v>
       </c>
       <c r="C75" t="s">
-        <v>137</v>
+        <v>160</v>
       </c>
       <c r="D75">
         <v>2800</v>
@@ -2812,13 +2890,13 @@
     </row>
     <row r="76" spans="1:9">
       <c r="A76" t="s">
-        <v>151</v>
-      </c>
-      <c r="B76">
-        <v>45209</v>
+        <v>176</v>
+      </c>
+      <c r="B76" t="s">
+        <v>23</v>
       </c>
       <c r="C76" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D76">
         <v>23280.5</v>
@@ -2826,13 +2904,13 @@
     </row>
     <row r="77" spans="1:9">
       <c r="A77" t="s">
-        <v>152</v>
-      </c>
-      <c r="B77">
-        <v>45232</v>
+        <v>177</v>
+      </c>
+      <c r="B77" t="s">
+        <v>170</v>
       </c>
       <c r="C77" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="D77">
         <v>246.02</v>
@@ -2840,13 +2918,13 @@
     </row>
     <row r="78" spans="1:9">
       <c r="A78" t="s">
-        <v>153</v>
-      </c>
-      <c r="B78">
-        <v>45231</v>
+        <v>178</v>
+      </c>
+      <c r="B78" t="s">
+        <v>168</v>
       </c>
       <c r="C78" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D78">
         <v>5901.48</v>
@@ -2854,13 +2932,13 @@
     </row>
     <row r="79" spans="1:9">
       <c r="A79" t="s">
-        <v>154</v>
-      </c>
-      <c r="B79">
-        <v>45203</v>
+        <v>179</v>
+      </c>
+      <c r="B79" t="s">
+        <v>10</v>
       </c>
       <c r="C79" t="s">
-        <v>155</v>
+        <v>180</v>
       </c>
       <c r="D79">
         <v>14636.18</v>
@@ -2868,13 +2946,13 @@
     </row>
     <row r="80" spans="1:9">
       <c r="A80" t="s">
-        <v>156</v>
-      </c>
-      <c r="B80">
-        <v>45218</v>
+        <v>181</v>
+      </c>
+      <c r="B80" t="s">
+        <v>49</v>
       </c>
       <c r="C80" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="D80">
         <v>1325</v>
@@ -2882,13 +2960,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>157</v>
-      </c>
-      <c r="B81">
-        <v>45200</v>
+        <v>182</v>
+      </c>
+      <c r="B81" t="s">
+        <v>110</v>
       </c>
       <c r="C81" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="D81">
         <v>7000</v>
@@ -2896,13 +2974,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>158</v>
-      </c>
-      <c r="B82">
-        <v>45201</v>
+        <v>183</v>
+      </c>
+      <c r="B82" t="s">
+        <v>7</v>
       </c>
       <c r="C82" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D82">
         <v>1901.24</v>
@@ -2910,13 +2988,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" t="s">
-        <v>159</v>
-      </c>
-      <c r="B83">
-        <v>45200</v>
+        <v>184</v>
+      </c>
+      <c r="B83" t="s">
+        <v>110</v>
       </c>
       <c r="C83" t="s">
-        <v>137</v>
+        <v>160</v>
       </c>
       <c r="D83">
         <v>-9849</v>
@@ -2924,13 +3002,13 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" t="s">
-        <v>160</v>
-      </c>
-      <c r="B84">
-        <v>45201</v>
+        <v>185</v>
+      </c>
+      <c r="B84" t="s">
+        <v>7</v>
       </c>
       <c r="C84" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D84">
         <v>904.5</v>
@@ -2938,13 +3016,13 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" t="s">
-        <v>161</v>
-      </c>
-      <c r="B85">
-        <v>45232</v>
+        <v>186</v>
+      </c>
+      <c r="B85" t="s">
+        <v>170</v>
       </c>
       <c r="C85" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D85">
         <v>17800</v>
@@ -2952,13 +3030,13 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" t="s">
-        <v>162</v>
-      </c>
-      <c r="B86">
-        <v>45224</v>
+        <v>187</v>
+      </c>
+      <c r="B86" t="s">
+        <v>28</v>
       </c>
       <c r="C86" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D86">
         <v>1969</v>
@@ -2966,13 +3044,13 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" t="s">
-        <v>163</v>
-      </c>
-      <c r="B87">
-        <v>45225</v>
+        <v>188</v>
+      </c>
+      <c r="B87" t="s">
+        <v>120</v>
       </c>
       <c r="C87" t="s">
-        <v>143</v>
+        <v>166</v>
       </c>
       <c r="D87">
         <v>2485</v>
@@ -2980,13 +3058,13 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" t="s">
-        <v>164</v>
-      </c>
-      <c r="B88">
-        <v>45209</v>
+        <v>189</v>
+      </c>
+      <c r="B88" t="s">
+        <v>23</v>
       </c>
       <c r="C88" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D88">
         <v>444.7</v>
@@ -2994,13 +3072,13 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" t="s">
-        <v>165</v>
-      </c>
-      <c r="B89">
-        <v>45200</v>
+        <v>190</v>
+      </c>
+      <c r="B89" t="s">
+        <v>110</v>
       </c>
       <c r="C89" t="s">
-        <v>137</v>
+        <v>160</v>
       </c>
       <c r="D89">
         <v>-37438.65</v>
@@ -3008,13 +3086,13 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" t="s">
-        <v>166</v>
-      </c>
-      <c r="B90">
-        <v>45200</v>
+        <v>191</v>
+      </c>
+      <c r="B90" t="s">
+        <v>110</v>
       </c>
       <c r="C90" t="s">
-        <v>167</v>
+        <v>192</v>
       </c>
       <c r="D90">
         <v>-1074.21</v>
@@ -3022,13 +3100,13 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" t="s">
-        <v>168</v>
-      </c>
-      <c r="B91">
-        <v>45218</v>
+        <v>193</v>
+      </c>
+      <c r="B91" t="s">
+        <v>49</v>
       </c>
       <c r="C91" t="s">
-        <v>169</v>
+        <v>194</v>
       </c>
       <c r="D91">
         <v>13268.61</v>

</xml_diff>

<commit_message>
Working generation of excel with no leftover transactions. integration test Passed
</commit_message>
<xml_diff>
--- a/tests/output_tests_data/transactions_output.xlsx
+++ b/tests/output_tests_data/transactions_output.xlsx
@@ -34,7 +34,7 @@
     <t>Amount</t>
   </si>
   <si>
-    <t>fc175bb6-0434-42ba-88f5-ea9791d39e8a</t>
+    <t>db6a8eb2-20de-4d5a-ae67-46df3e26c3ce</t>
   </si>
   <si>
     <t>10-02-2023</t>
@@ -43,13 +43,13 @@
     <t>clover</t>
   </si>
   <si>
-    <t>927eded4-3cd1-4349-90c3-eae7a861b3e2</t>
+    <t>378735b5-5969-45ee-a2ba-cf0fd2b135ea</t>
   </si>
   <si>
     <t>Preauthorized Credit</t>
   </si>
   <si>
-    <t>19ac575f-8939-4374-9f9e-0924e0a7a7e5</t>
+    <t>39744341-d997-4116-8236-032c04ecd690</t>
   </si>
   <si>
     <t>10-01-2023</t>
@@ -58,49 +58,49 @@
     <t>rfms</t>
   </si>
   <si>
-    <t>64ac8ecb-8c2d-4705-a9b1-e6c7d28b79b2</t>
-  </si>
-  <si>
-    <t>d45368af-56fa-4c5c-9452-4210385927a4</t>
+    <t>61f873fe-ee69-4a62-b9e7-d098d5df89f8</t>
+  </si>
+  <si>
+    <t>d118e741-c894-4514-bbf2-c7e99e98fbde</t>
   </si>
   <si>
     <t>Amerigroup</t>
   </si>
   <si>
-    <t>fb824d4f-f3b2-4d04-9753-b2b694a673c6</t>
+    <t>1019da29-266e-4375-ada0-69a1bbaa7f10</t>
   </si>
   <si>
     <t>10-04-2023</t>
   </si>
   <si>
-    <t>dad1b938-ee3c-4dd5-b986-43d5bcf43df6</t>
+    <t>80135c99-cf11-4679-9bd1-37ea7701b7a5</t>
   </si>
   <si>
     <t>uhc</t>
   </si>
   <si>
-    <t>4e60630f-fc95-4d78-a80a-e73a22889877</t>
-  </si>
-  <si>
-    <t>472e9755-ca5b-4205-b008-b4c7f297e7c7</t>
+    <t>da3d5b66-1086-4662-8cf1-ae13ff1af947</t>
+  </si>
+  <si>
+    <t>96210550-819f-4f68-89a6-2876189c7407</t>
   </si>
   <si>
     <t>Horizon NJ Health</t>
   </si>
   <si>
-    <t>219f7302-892c-4391-88d6-73f50c284b02</t>
-  </si>
-  <si>
-    <t>a0dabcac-f772-4882-93b1-969579a9f424</t>
+    <t>758a5a11-b7bb-4282-8a5f-229b33425904</t>
+  </si>
+  <si>
+    <t>317397df-ca4e-48ca-b288-81141ef8ae39</t>
   </si>
   <si>
     <t>10-03-2023</t>
   </si>
   <si>
-    <t>5245a5dc-e9ad-4a85-aa48-02b324134632</t>
-  </si>
-  <si>
-    <t>50ceb500-68c5-4c78-9c72-270b55d0d2c5</t>
+    <t>9da5361d-e75c-45b3-83e7-c260bd7ca9f1</t>
+  </si>
+  <si>
+    <t>b7ab5476-602d-44db-8a22-f1aa4f3cb8f7</t>
   </si>
   <si>
     <t>10-05-2023</t>
@@ -109,592 +109,592 @@
     <t>fidelis</t>
   </si>
   <si>
-    <t>b2797b42-51e6-4816-a5f4-d0fa3f5b47d1</t>
-  </si>
-  <si>
-    <t>f80ba2f1-298e-4ee6-b8e9-74c60e25119a</t>
-  </si>
-  <si>
-    <t>82753ae9-d087-4f9a-9608-c6fa1ecba921</t>
-  </si>
-  <si>
-    <t>99c45fd3-f3e8-4783-996d-5cb550622356</t>
-  </si>
-  <si>
-    <t>e7a8d9f2-9f57-44b7-b92a-c97fa8b575fa</t>
-  </si>
-  <si>
-    <t>2b63204e-1f5e-4eba-aacc-abd18d820421</t>
+    <t>78d008e6-41b0-4cd0-a291-a48b7c778c70</t>
+  </si>
+  <si>
+    <t>de2d6a87-00cf-4bc1-b3f7-3fcdc58d8ea2</t>
+  </si>
+  <si>
+    <t>583c9543-19bd-4353-b805-9da8774a876f</t>
+  </si>
+  <si>
+    <t>3d06529a-bedb-4467-be51-a5c05d8ecc89</t>
+  </si>
+  <si>
+    <t>1610aa97-2ba8-4282-919e-9c59a31ecd31</t>
+  </si>
+  <si>
+    <t>7f80c88f-d0d6-495c-94e3-294f38df590b</t>
   </si>
   <si>
     <t>10-06-2023</t>
   </si>
   <si>
-    <t>4143e8ce-d695-44e0-a918-407249b9eea7</t>
-  </si>
-  <si>
-    <t>c4f6e86c-14a4-4746-ab98-8fabf83888fb</t>
+    <t>ff52c4b8-3234-4377-9294-4fa4e0f35f01</t>
+  </si>
+  <si>
+    <t>207a823e-120f-438e-9480-d2e527463e99</t>
   </si>
   <si>
     <t>facility deposit</t>
   </si>
   <si>
-    <t>debb5245-374f-4545-aae2-817f3a1b5c14</t>
+    <t>4a41e666-9a99-457c-a77e-e494f438c72e</t>
   </si>
   <si>
     <t>Remote Deposit</t>
   </si>
   <si>
-    <t>ab562282-ed1a-4d7f-919f-c17643bc1935</t>
+    <t>2273dabf-1630-4215-9781-22ea5cc58410</t>
   </si>
   <si>
     <t>10-10-2023</t>
   </si>
   <si>
-    <t>b416d533-7f9d-4ea9-a8c1-b21d126c2bfd</t>
-  </si>
-  <si>
-    <t>a8ef9928-0f29-4bae-9b2d-86b70fada898</t>
-  </si>
-  <si>
-    <t>cfa3989b-eaf8-40d8-8de1-858c50d59999</t>
-  </si>
-  <si>
-    <t>41e54657-2c5a-4329-ac0a-dd9b6e1483e1</t>
+    <t>cca83a91-c752-431e-bbba-f9d9e3d68601</t>
+  </si>
+  <si>
+    <t>95ec188d-ed8a-4951-b1bc-88607fe6b853</t>
+  </si>
+  <si>
+    <t>f26acf84-228b-468a-8a4a-84d42021a31b</t>
+  </si>
+  <si>
+    <t>148a9d85-444a-4ef8-adf6-ff94b648f171</t>
   </si>
   <si>
     <t>10-08-2023</t>
   </si>
   <si>
-    <t>5f2f07d7-39fa-41b0-8e01-4abefd09fee1</t>
-  </si>
-  <si>
-    <t>ac365245-e985-4e8f-b25b-54ff20299268</t>
+    <t>45b87275-767a-4557-97a7-57ce75bad14c</t>
+  </si>
+  <si>
+    <t>3468f9be-813e-44d6-ae04-e4d921315340</t>
   </si>
   <si>
     <t>Aetna Better Health</t>
   </si>
   <si>
-    <t>9889e3bf-d738-4373-9242-77ee85b15b77</t>
-  </si>
-  <si>
-    <t>c9d60105-10f0-469f-87b8-403c284139a6</t>
+    <t>c2b1f9bd-04c2-4e22-8652-c4c0debc69ec</t>
+  </si>
+  <si>
+    <t>2d56828f-5434-4870-8942-4a21889b00bd</t>
   </si>
   <si>
     <t>10-11-2023</t>
   </si>
   <si>
-    <t>f5c4952c-dfb8-4926-adad-b19a9a751256</t>
-  </si>
-  <si>
-    <t>997358a3-30e1-44c2-b08f-fcd184afbc4d</t>
+    <t>ef8e3abc-ea51-42ad-86aa-221f7680d02d</t>
+  </si>
+  <si>
+    <t>0a918546-a403-426c-8807-28818821f2a9</t>
   </si>
   <si>
     <t>10-09-2023</t>
   </si>
   <si>
-    <t>360eb0af-4ac0-4df9-bca4-dc14fb99eec5</t>
-  </si>
-  <si>
-    <t>eb5ab619-1e57-4d47-81d4-79b5cb99786f</t>
-  </si>
-  <si>
-    <t>211ebe18-af17-4e4f-8b84-24f072e9f7f4</t>
-  </si>
-  <si>
-    <t>0da8c76b-c77d-4f0b-989e-733d090ae400</t>
+    <t>b2497c04-aa83-49e6-9133-a6ce4daf6125</t>
+  </si>
+  <si>
+    <t>a54cc493-c497-4b36-978e-596140cda202</t>
+  </si>
+  <si>
+    <t>d35a3628-7875-4efb-ab17-2cc79289c8d0</t>
+  </si>
+  <si>
+    <t>b2f6e9a5-ce3b-441a-a550-ea929dd9cd97</t>
   </si>
   <si>
     <t>10-12-2023</t>
   </si>
   <si>
-    <t>f3463ff8-8e9d-4b03-914e-e7c270211fcc</t>
-  </si>
-  <si>
-    <t>5524242c-ecb9-40e9-99b4-075ca9e973e3</t>
-  </si>
-  <si>
-    <t>136d8dd3-9c67-4e9c-8dd8-a82ab7ed2731</t>
-  </si>
-  <si>
-    <t>aa62b697-e086-4460-8d33-4b7d4dc51f01</t>
-  </si>
-  <si>
-    <t>d5dc5162-7def-4f2f-953c-bcde383ce9af</t>
-  </si>
-  <si>
-    <t>e6173d52-77c1-4ca0-9d49-31df8a6e321f</t>
-  </si>
-  <si>
-    <t>d2f8ac0d-c4a7-4616-82e4-9ced02cdceff</t>
-  </si>
-  <si>
-    <t>4fbcac63-3337-43c3-a0aa-bca58f7ea5ca</t>
+    <t>bb31aa7e-9cca-4594-9116-a65228c7d2db</t>
+  </si>
+  <si>
+    <t>6d1e6923-8a04-49a3-84a3-9b8aaa8d6ae3</t>
+  </si>
+  <si>
+    <t>54c3b93c-df11-4fce-b565-30168ea5da71</t>
+  </si>
+  <si>
+    <t>3912b2ab-3409-4bea-b237-fc46da214393</t>
+  </si>
+  <si>
+    <t>1bbae743-67c3-4388-89b2-e077a772c6bc</t>
+  </si>
+  <si>
+    <t>4615339c-ecfe-4b29-9ec0-4ac5cc327df0</t>
+  </si>
+  <si>
+    <t>002d4a01-cdec-4bb5-bc71-cc16d7b364e6</t>
+  </si>
+  <si>
+    <t>da7cffce-2b7f-45e3-8d0d-89d82950c8d5</t>
   </si>
   <si>
     <t>10-13-2023</t>
   </si>
   <si>
-    <t>e373453d-560f-4eb5-bcdd-9cce49c16853</t>
-  </si>
-  <si>
-    <t>92ac9670-7427-49f7-a07f-6d432fe94a90</t>
+    <t>d8450ee1-78b3-43f2-ab11-88a06984cd74</t>
+  </si>
+  <si>
+    <t>3bb7a029-4d4c-4da5-8bba-f7b11ebb8246</t>
   </si>
   <si>
     <t>10-16-2023</t>
   </si>
   <si>
-    <t>93bf3160-0fd4-4340-8c25-fff066a2c680</t>
-  </si>
-  <si>
-    <t>725e6ef3-c01a-4ec1-89c5-fa9a1cb18b44</t>
-  </si>
-  <si>
-    <t>74e286a7-05a8-47c8-8214-e222b2c115ba</t>
-  </si>
-  <si>
-    <t>ed091454-70be-4549-b8e1-3fb6f006ca75</t>
-  </si>
-  <si>
-    <t>fb8dc8d1-27ed-436b-8d3f-113b260359c1</t>
-  </si>
-  <si>
-    <t>e7078ab6-b4ac-4cc5-bea4-9df83bffeaf0</t>
+    <t>b6e90e65-61cf-418c-836f-5bfce3135ad3</t>
+  </si>
+  <si>
+    <t>87ef5479-152d-497e-81a9-169365af9ecb</t>
+  </si>
+  <si>
+    <t>e5ee28e2-e97a-4f71-b81b-375a3ac1c458</t>
+  </si>
+  <si>
+    <t>3d36f19d-2446-4ac0-81cb-30b54406c631</t>
+  </si>
+  <si>
+    <t>d6cc38ca-4f99-4270-8959-f3a5d3428a32</t>
+  </si>
+  <si>
+    <t>8f1f8611-3f49-40fb-8b30-7e01cc0bea9f</t>
   </si>
   <si>
     <t>10-17-2023</t>
   </si>
   <si>
-    <t>faea74a3-6d81-4506-9015-fd43f7b24efb</t>
-  </si>
-  <si>
-    <t>70bf8336-9178-4772-8f62-ae740053fa33</t>
+    <t>d5286dbe-d1ea-4e00-b01a-a94279f624ce</t>
+  </si>
+  <si>
+    <t>96c928a1-73e6-403d-8687-adec82bd080c</t>
   </si>
   <si>
     <t>10-24-2023</t>
   </si>
   <si>
-    <t>4f5ad6a2-b96d-4c7e-9287-d4c6cf89c9ed</t>
-  </si>
-  <si>
-    <t>4c509d66-6f2e-4036-8d59-5c8fabe45a42</t>
-  </si>
-  <si>
-    <t>8f9312a3-33af-4726-bc72-54081216a9db</t>
-  </si>
-  <si>
-    <t>a8469c51-8bf5-4df8-bcfd-f13c47de0834</t>
-  </si>
-  <si>
-    <t>cb4dd4a0-9a66-4a76-b62f-9baf2e4ea127</t>
-  </si>
-  <si>
-    <t>5fb96955-23b3-4f14-ac8f-5a9ea6a06be2</t>
+    <t>0acaba83-2858-4037-b94c-7f91402be52f</t>
+  </si>
+  <si>
+    <t>5e326181-e482-4211-a019-05e51050a240</t>
+  </si>
+  <si>
+    <t>a64ca065-38cb-46f9-a639-9102d8e8b592</t>
+  </si>
+  <si>
+    <t>9b88948a-ba7d-465a-ba78-088eae33e08e</t>
+  </si>
+  <si>
+    <t>57d430d5-0813-47a0-885f-22439d3700f2</t>
+  </si>
+  <si>
+    <t>ccc92efc-8caa-4d8c-8dfd-c6e7a5d1ffea</t>
   </si>
   <si>
     <t>credit card</t>
   </si>
   <si>
-    <t>5204f2ea-a04a-422a-ae46-9464495d885d</t>
-  </si>
-  <si>
-    <t>66c02c64-6888-4d02-b466-1faa2ab9537c</t>
-  </si>
-  <si>
-    <t>220d93b7-2864-4a94-9c9e-486b0a5538a1</t>
-  </si>
-  <si>
-    <t>e8f833d7-92a0-4344-b8e5-15cb0f640ea6</t>
+    <t>42731a43-7605-4870-938f-c3d18c726b9e</t>
+  </si>
+  <si>
+    <t>cf6008db-0629-4ba7-933c-dc538e8610bb</t>
+  </si>
+  <si>
+    <t>edc268df-2ae9-4463-86ec-23f6d4b2a128</t>
+  </si>
+  <si>
+    <t>d9366f65-a5ed-4984-b6c5-3ece1b10818f</t>
   </si>
   <si>
     <t>facility depost</t>
   </si>
   <si>
-    <t>3aed358c-9240-4632-8113-0d12b6c472f4</t>
-  </si>
-  <si>
-    <t>89350510-1473-459b-b200-610c61e36b5a</t>
+    <t>e22767eb-5f1e-42e9-b677-85c48dc5a26b</t>
+  </si>
+  <si>
+    <t>3931a353-b34d-4cab-8176-a6d2cd70b960</t>
   </si>
   <si>
     <t>10-18-2023</t>
   </si>
   <si>
-    <t>bc0e9e63-515f-434c-98f4-1abf5bfa2ee6</t>
-  </si>
-  <si>
-    <t>43d950d0-fd1e-4968-b163-1f93e4b4ee3f</t>
-  </si>
-  <si>
-    <t>cf53d42b-6d3d-4d50-9e37-b3c30a9f336b</t>
-  </si>
-  <si>
-    <t>31f8da4a-bf3a-4122-bd08-b0354a1f14a6</t>
-  </si>
-  <si>
-    <t>8a8fa0a0-a533-4618-8fc2-4ac935d0d4ce</t>
-  </si>
-  <si>
-    <t>08d569ce-9af2-4712-8c41-9da76cdc5fed</t>
-  </si>
-  <si>
-    <t>66695b0d-fcb2-4d53-aaa3-0b8197f67049</t>
+    <t>a40246cf-08ab-4bd9-b08c-79067df4041f</t>
+  </si>
+  <si>
+    <t>65b9fd4a-aa9d-4a75-b12f-65a55c098978</t>
+  </si>
+  <si>
+    <t>5759e315-a58d-4bac-b9f5-5516a307e470</t>
+  </si>
+  <si>
+    <t>45f00677-37f8-4b2a-80c6-04f62f6d107e</t>
+  </si>
+  <si>
+    <t>12a7fab5-98d8-437a-ae18-2cfb3fbfca96</t>
+  </si>
+  <si>
+    <t>f212c7d9-e93a-4bcb-a5c9-c07f6819322b</t>
+  </si>
+  <si>
+    <t>073cba62-73c2-4f78-945e-0b8834b5b2fd</t>
   </si>
   <si>
     <t>10-19-2023</t>
   </si>
   <si>
-    <t>6da70d4a-ec4b-4f8a-a6a8-b9c325a94638</t>
+    <t>5065bb5c-b457-46e4-b513-e34824ae1758</t>
   </si>
   <si>
     <t>optum roster</t>
   </si>
   <si>
-    <t>882cf11b-32c0-4fb2-8292-fdd444818868</t>
-  </si>
-  <si>
-    <t>ad858718-f2a7-4556-afbb-cf2afd3363ce</t>
-  </si>
-  <si>
-    <t>fbfad492-5789-48bc-affe-b638f76ab396</t>
-  </si>
-  <si>
-    <t>bb250da8-5dea-4bbd-adf1-78a3ef33b31d</t>
-  </si>
-  <si>
-    <t>ce4b7195-1d81-45c4-bc60-2c7c558a76b2</t>
+    <t>42b57061-6416-4cef-854f-499292baacb1</t>
+  </si>
+  <si>
+    <t>31e0467e-91c5-470c-854d-d5c9334fe4e0</t>
+  </si>
+  <si>
+    <t>9a0a9bb2-f317-4b7b-b19e-71942d6f1279</t>
+  </si>
+  <si>
+    <t>d984ccb8-ef65-47a2-8335-b62d5c8fa71d</t>
+  </si>
+  <si>
+    <t>46f930f9-09c9-47b1-9c56-40c54fb64307</t>
   </si>
   <si>
     <t>10-20-2023</t>
   </si>
   <si>
-    <t>0c9b8915-ae29-4e46-9a2f-e3fbb177eb06</t>
+    <t>e594c91f-bdc4-4e78-a962-88c673db2f2b</t>
   </si>
   <si>
     <t>10-23-2023</t>
   </si>
   <si>
-    <t>7106b225-ba43-4730-b908-6857e80778d8</t>
-  </si>
-  <si>
-    <t>0660958a-b684-4777-975d-0307950d760d</t>
-  </si>
-  <si>
-    <t>58066222-6500-4761-9038-438462bc20e3</t>
-  </si>
-  <si>
-    <t>56433262-49a7-42cc-ba45-8f732c4b96d3</t>
-  </si>
-  <si>
-    <t>0f5b7ede-8a77-479c-9c05-6a74d4fa43ea</t>
-  </si>
-  <si>
-    <t>ba5d69c0-3559-426c-b175-fe6c12093600</t>
+    <t>e311bbc0-cca8-4b56-985c-1e2d880c17e4</t>
+  </si>
+  <si>
+    <t>7a6ac5b1-a206-4453-9f66-a8e781bf5cd4</t>
+  </si>
+  <si>
+    <t>57736727-a2fb-4cb5-a4a2-e305c8f9b74d</t>
+  </si>
+  <si>
+    <t>14fea3cc-645f-4bb1-802d-359b81768fae</t>
+  </si>
+  <si>
+    <t>4febe88c-7b58-48da-a81c-b05880b7f895</t>
+  </si>
+  <si>
+    <t>9b268d92-9e6e-4cb6-8a64-4538ddcd5f08</t>
   </si>
   <si>
     <t>10-25-2023</t>
   </si>
   <si>
-    <t>b07f5e34-61b6-457b-b581-a4bdcc3f5971</t>
-  </si>
-  <si>
-    <t>cbdd2b7d-891c-4b12-854b-de073fb69e40</t>
-  </si>
-  <si>
-    <t>6b44ed30-914a-4620-a57a-d562b93bbc81</t>
-  </si>
-  <si>
-    <t>b02caa60-4f53-470b-a11e-9e0761561041</t>
-  </si>
-  <si>
-    <t>e6d20c0c-e4f5-449b-8c61-5fecf68cd6e4</t>
-  </si>
-  <si>
-    <t>830cb2fe-3090-44a7-bf72-3d806bb7c5eb</t>
+    <t>52d103fa-11fe-4d0a-ae6d-c9b02755ebc1</t>
+  </si>
+  <si>
+    <t>9523e284-841e-4a2a-9f0d-dbdd813c6263</t>
+  </si>
+  <si>
+    <t>c3a0ed97-db97-429d-be16-0fbb6ddf8227</t>
+  </si>
+  <si>
+    <t>cd89f8d2-824d-448d-8ec6-62ef90d2d193</t>
+  </si>
+  <si>
+    <t>6efe531f-5e76-4372-9498-19fac33ac052</t>
+  </si>
+  <si>
+    <t>0489cbd8-c444-4fcf-bd81-9f914f6fe6fe</t>
   </si>
   <si>
     <t>10-26-2023</t>
   </si>
   <si>
-    <t>f88418d7-5e33-49a7-b08f-805f73dd43a7</t>
-  </si>
-  <si>
-    <t>5e6cf59c-f0c9-43eb-ac68-84221111aea8</t>
+    <t>540f2ab5-8ca5-4769-866d-898ce78d1c32</t>
+  </si>
+  <si>
+    <t>e6036433-b41c-4b6e-b851-c7e19542e97f</t>
   </si>
   <si>
     <t>10-30-2023</t>
   </si>
   <si>
-    <t>f98272df-71b6-4266-a8dd-b64d287549e4</t>
-  </si>
-  <si>
-    <t>ece0ce83-1227-486d-8aeb-4be3e893c442</t>
-  </si>
-  <si>
-    <t>b02e19d9-47db-4b34-835c-fb4aa7eb04c4</t>
-  </si>
-  <si>
-    <t>ba59f4d9-72c6-42d8-ab0b-8e067ecf2a71</t>
+    <t>b188d561-7a38-4cba-bdb2-72b5c363624d</t>
+  </si>
+  <si>
+    <t>be9e5a4e-39af-424e-9687-5640d3d9198d</t>
+  </si>
+  <si>
+    <t>0c79ca7a-83ad-4480-98ea-dfa013c82439</t>
+  </si>
+  <si>
+    <t>9b54ac2c-c940-486d-bb78-c8a46af1c00e</t>
   </si>
   <si>
     <t>10-31-2023</t>
   </si>
   <si>
-    <t>7d194d5e-5355-4e47-9d9e-207308830119</t>
-  </si>
-  <si>
-    <t>0f42c4dd-978a-43e8-b823-5e0f9085f237</t>
-  </si>
-  <si>
-    <t>8b24a76b-5494-4452-9e90-79db63c730b3</t>
-  </si>
-  <si>
-    <t>e0f5dc5f-d70d-4b20-aa63-445e1e4c57ab</t>
-  </si>
-  <si>
-    <t>24dd7cc5-0846-4baa-b9f4-d4d3772a7d1c</t>
+    <t>fcd06d17-d5ed-4f3e-95c4-c77bdba1aec7</t>
+  </si>
+  <si>
+    <t>83ce1397-3f8a-48a1-9fb9-52ea9e0676d1</t>
+  </si>
+  <si>
+    <t>6cf63010-e4d0-4464-9a21-b7ee6f4a6ef7</t>
+  </si>
+  <si>
+    <t>358d5827-97a7-48da-8b3f-6740bba3e59c</t>
+  </si>
+  <si>
+    <t>cdceb4df-1216-41b8-a187-6c73979711dd</t>
   </si>
   <si>
     <t>humana cc</t>
   </si>
   <si>
-    <t>3d51364b-586d-427f-8730-ff2490410ff8</t>
-  </si>
-  <si>
-    <t>4d1fc1d4-3017-4881-a4d7-606f7be63e4b</t>
+    <t>9cdc731e-b032-4edc-874b-012d62d4e308</t>
+  </si>
+  <si>
+    <t>7f3913e3-7767-46c9-9697-7b094e177b8d</t>
   </si>
   <si>
     <t>wellmed cc</t>
   </si>
   <si>
-    <t>886b237d-12de-4ecc-a191-5908ff4a01b0</t>
-  </si>
-  <si>
-    <t>d5da19b2-6e66-45c1-9922-42d49d0e2ed0</t>
+    <t>71b94f39-3c59-44ee-86d4-c5801984e785</t>
+  </si>
+  <si>
+    <t>918cea4a-ad38-4763-9b32-627b6cf9f908</t>
   </si>
   <si>
     <t>uhc cc</t>
   </si>
   <si>
-    <t>07fbe688-702f-472d-bab2-bdacd2bf70f1</t>
-  </si>
-  <si>
-    <t>64733d74-ef9b-4ef3-aa04-a97c99c8a563</t>
-  </si>
-  <si>
-    <t>0f714db0-ba7e-4928-8ace-f9ecbcc05c8a</t>
+    <t>1c405927-429b-40fb-9098-7e018f8b5342</t>
+  </si>
+  <si>
+    <t>ddfa532f-f260-4118-b629-a19c09462043</t>
+  </si>
+  <si>
+    <t>14967100-cfff-4d3c-9dca-b3d49affdf2d</t>
   </si>
   <si>
     <t>10-27-2023</t>
   </si>
   <si>
-    <t>3a9c0e3e-0c18-4323-a1a2-e6ebb5db3fc9</t>
-  </si>
-  <si>
-    <t>c49d9b64-53fe-4c27-878e-557e1dbadf33</t>
+    <t>9708bbf8-8256-4f42-9db1-b3d909192da4</t>
+  </si>
+  <si>
+    <t>7ba4cac0-3de2-4e5f-ad2a-dec0b2c8bea5</t>
   </si>
   <si>
     <t>RFMS</t>
   </si>
   <si>
-    <t>07b50205-50bb-4b13-9cbd-6426c2302c60</t>
-  </si>
-  <si>
-    <t>509b55ab-51b2-478c-9c65-1ffe4731007b</t>
+    <t>3916bf8e-b430-4d2f-b5cb-baa3c45fc098</t>
+  </si>
+  <si>
+    <t>c49fd2c0-0782-41c8-9cb3-3197277fa19b</t>
   </si>
   <si>
     <t>cigna cc</t>
   </si>
   <si>
-    <t>8cc69950-d41e-4f58-a0eb-7b294e56928d</t>
+    <t>7bdc2e2b-afcb-4151-b6f1-2ef6822d18e3</t>
   </si>
   <si>
     <t>11-01-2023</t>
   </si>
   <si>
-    <t>de5b0db1-792d-410c-bb5a-6c1bc2e2a5ec</t>
+    <t>efa070d9-7be7-416d-b1b9-17253fef2844</t>
   </si>
   <si>
     <t>gnss wire</t>
   </si>
   <si>
-    <t>9b0cd803-4ead-42d6-97c0-6eb4edb53bba</t>
-  </si>
-  <si>
-    <t>bf831c52-9bc0-4f4e-8c04-14d37e6f29e1</t>
+    <t>b2e6f0d0-cf12-4014-8e82-060237a3e70b</t>
+  </si>
+  <si>
+    <t>63645430-8cf8-45c8-90b7-1cbba55d0d56</t>
   </si>
   <si>
     <t>gen wire</t>
   </si>
   <si>
-    <t>6f2f4ddb-5203-49f4-b31c-736ee05cc5a4</t>
+    <t>487a74bb-fb3d-457f-b9ad-552191ba6f3d</t>
   </si>
   <si>
     <t>wire</t>
   </si>
   <si>
-    <t>242be4ba-22da-454e-b168-803401c6528e</t>
-  </si>
-  <si>
-    <t>7eb72a13-9bab-497e-bf05-b3f63846285e</t>
-  </si>
-  <si>
-    <t>e975e6d7-3493-4d4e-84cc-4a74f799c25c</t>
-  </si>
-  <si>
-    <t>b1e625ee-0c7c-4dba-a6f7-de70b96e5565</t>
+    <t>29fa2e20-a7a5-40b8-bf9d-e5ff06f62d74</t>
+  </si>
+  <si>
+    <t>262cefec-3740-4990-a337-8168409f0360</t>
+  </si>
+  <si>
+    <t>e20cb283-06c0-4f04-9b9a-3daf5d6fd6f7</t>
+  </si>
+  <si>
+    <t>6709c14f-8f53-4cb4-9d40-da46b19e2b40</t>
   </si>
   <si>
     <t>gnss wire back up</t>
   </si>
   <si>
-    <t>7b41e538-e282-4658-a167-5c228ce46365</t>
+    <t>1ea699e6-f41c-4938-81d9-89e8468b17cd</t>
   </si>
   <si>
     <t>genesis wire 10/5/23 backup</t>
   </si>
   <si>
-    <t>3d64bc7a-2dfe-4307-b3d4-44cd56e2b6d2</t>
+    <t>3258345a-998a-43d7-b95a-679a82fa777b</t>
   </si>
   <si>
     <t>adjustments</t>
   </si>
   <si>
-    <t>17e6aeab-264e-4390-b6b8-9a329d568421</t>
+    <t>18dc5f80-2fb5-40e1-91de-a6acd585d5ec</t>
   </si>
   <si>
     <t>write off</t>
   </si>
   <si>
-    <t>e1a1fe89-5d80-4c5f-b708-59e48cae72e9</t>
+    <t>b472a35d-1896-4058-a036-e709c4ead1ae</t>
   </si>
   <si>
     <t>writeoff</t>
   </si>
   <si>
-    <t>98c3b9e0-c6ac-497a-98e4-b6d13843c99b</t>
-  </si>
-  <si>
-    <t>225ff7c7-4741-4285-86ad-2a70f3a58ced</t>
+    <t>b8b4e79d-2cbf-4d19-b3e9-ab8186a8b944</t>
+  </si>
+  <si>
+    <t>52ce5d15-ba06-4b32-b138-b50dfb97a2b5</t>
   </si>
   <si>
     <t>gnss wire 9/5/23</t>
   </si>
   <si>
-    <t>a7994ae9-1f37-4af9-95ef-299593a8b91c</t>
-  </si>
-  <si>
-    <t>414950dd-df28-4d8a-bc99-975407adc58f</t>
-  </si>
-  <si>
-    <t>9a6c23c8-288b-4d40-a445-57e8dcf82191</t>
-  </si>
-  <si>
-    <t>85a0e55a-860d-4926-95b8-0d773432c00f</t>
-  </si>
-  <si>
-    <t>9b18c958-086b-4b40-aa95-58a2ab9958f7</t>
+    <t>b8a2dcae-c737-450b-9c46-a51827b88a4f</t>
+  </si>
+  <si>
+    <t>b5256fbe-0862-4989-a185-ff6ab290c074</t>
+  </si>
+  <si>
+    <t>c552bab5-663c-4708-8d88-f08f76dd47b0</t>
+  </si>
+  <si>
+    <t>3fcead5b-455a-45e4-a544-da2f066c4933</t>
+  </si>
+  <si>
+    <t>f23d8fa3-2e33-497b-adc8-3be9b7d371e6</t>
   </si>
   <si>
     <t>hnjh ( total is 3681.72)</t>
   </si>
   <si>
-    <t>4930aa71-47b2-4384-afaf-5ea4925e80d6</t>
+    <t>af3eb4d5-1036-4845-8af6-a439891e7340</t>
   </si>
   <si>
     <t>genesis wire 10/5/23</t>
   </si>
   <si>
-    <t>e9c4bee5-bcd7-400e-bd1c-a7dd4d1703fc</t>
-  </si>
-  <si>
-    <t>b9b42bb3-33d7-4cab-a447-c1ffe85d29e6</t>
-  </si>
-  <si>
-    <t>11d3c87c-b56f-4141-b4aa-1ce133f7d639</t>
-  </si>
-  <si>
-    <t>45395847-8803-41d0-b7ff-387288c0ae3e</t>
-  </si>
-  <si>
-    <t>33dae0f0-a016-4fbc-bb0e-c9d24c0c45e1</t>
-  </si>
-  <si>
-    <t>3ed11a97-be26-46c6-9bd9-5858ea096fde</t>
-  </si>
-  <si>
-    <t>cecb91fc-b218-41e1-a89c-374dd05d36fc</t>
-  </si>
-  <si>
-    <t>69c4a177-19dc-471d-9e22-d0ce22ef8495</t>
-  </si>
-  <si>
-    <t>04170e75-0213-4cc4-86c6-40da5ffe1161</t>
-  </si>
-  <si>
-    <t>c7bc8f50-fd7e-4cac-8af9-3e9ef1f8f6db</t>
-  </si>
-  <si>
-    <t>ea600c0b-9138-40e1-ba91-1dd615d79a46</t>
-  </si>
-  <si>
-    <t>dd4a8db3-e668-432b-a637-49ae4ac3d09a</t>
-  </si>
-  <si>
-    <t>a567df7d-2ec3-41d3-9d1e-3c07e0c5489e</t>
+    <t>c1f13720-a3b5-4b4f-8af7-f6c1436f76fb</t>
+  </si>
+  <si>
+    <t>69081c3f-0b5c-4f84-96e1-97fa93b7fff5</t>
+  </si>
+  <si>
+    <t>ac0c0e36-619d-4294-b6bc-4e20b3b40842</t>
+  </si>
+  <si>
+    <t>fef84334-6bfd-4d0a-9a7b-1d33cd0ce776</t>
+  </si>
+  <si>
+    <t>a165668f-11bf-42c2-8a40-4946674986ef</t>
+  </si>
+  <si>
+    <t>23c4f119-36b9-4940-b899-fdafba12b72b</t>
+  </si>
+  <si>
+    <t>40e59629-3e0e-4153-9f4e-961b51a75150</t>
+  </si>
+  <si>
+    <t>defb22a9-a677-4841-ab37-7672aa9da28d</t>
+  </si>
+  <si>
+    <t>275c77d5-0bb2-48c4-887e-bb826af32469</t>
+  </si>
+  <si>
+    <t>10b2a1cc-08ea-4dde-b371-ee2e7135e8be</t>
+  </si>
+  <si>
+    <t>1ab31d69-66db-4d7b-ac3f-43b577b6f4fe</t>
+  </si>
+  <si>
+    <t>0efdaf14-d3a2-4960-8391-f3129f811565</t>
+  </si>
+  <si>
+    <t>959d989b-97be-4c8d-b308-61a7230bc191</t>
   </si>
   <si>
     <t>11-02-2023</t>
   </si>
   <si>
-    <t>b3d002de-d4bc-4b7d-b10c-70b822d688a6</t>
-  </si>
-  <si>
-    <t>881bfe20-dae3-47e4-86c4-840954501355</t>
-  </si>
-  <si>
-    <t>9561abd4-01df-4636-b39c-d3718acd719e</t>
-  </si>
-  <si>
-    <t>be914556-7ee7-4a75-8c9a-d6906c1e247e</t>
-  </si>
-  <si>
-    <t>694ba05c-32f4-484f-b0af-b508cfa7d262</t>
-  </si>
-  <si>
-    <t>6885c5df-3ed0-4319-8f3b-f133e78771e8</t>
-  </si>
-  <si>
-    <t>44bd3d7c-c5de-4a72-b4a5-4029c2a9ffde</t>
+    <t>35a6c52b-664e-49f9-8091-02a6cc2bb95c</t>
+  </si>
+  <si>
+    <t>fcc73fda-edce-4a71-b1c6-beec6306506a</t>
+  </si>
+  <si>
+    <t>851474c4-884e-4df5-9546-14fdc8c298d8</t>
+  </si>
+  <si>
+    <t>469c0dc1-46ea-43e8-b2ce-39efdb233d4d</t>
+  </si>
+  <si>
+    <t>524768b8-09e3-4ec8-9722-dae461aa72bd</t>
+  </si>
+  <si>
+    <t>484c539e-b820-4f08-9903-d6b4a3e8803b</t>
+  </si>
+  <si>
+    <t>5f0a6dd3-1e87-42ca-8fd5-423d70f25e58</t>
   </si>
   <si>
     <t>Automatic Transfer</t>
   </si>
   <si>
-    <t>67922c80-c1d7-4ce0-b3c8-03c7773f3856</t>
-  </si>
-  <si>
-    <t>4a5b6c76-d46a-4a1c-adbd-39cb26e04460</t>
-  </si>
-  <si>
-    <t>9e472234-d2f1-45e9-942f-c3e580fe5c35</t>
-  </si>
-  <si>
-    <t>564c4c42-5ac4-433b-abce-82ada0a6b2b9</t>
-  </si>
-  <si>
-    <t>5314d8fb-e406-4557-9413-86aa6228c1eb</t>
-  </si>
-  <si>
-    <t>21b3dfe7-38a7-4f1b-bf33-8444f304e167</t>
-  </si>
-  <si>
-    <t>99c03960-950d-4627-b097-31aca697ff3d</t>
-  </si>
-  <si>
-    <t>fbcaab18-78fa-42b2-af52-14fb97d3cb45</t>
-  </si>
-  <si>
-    <t>b2e3cc3d-6432-4ba4-9fa6-293d38fe4ff6</t>
+    <t>ef02cf46-7558-45b6-9daf-fff2d56cd06e</t>
+  </si>
+  <si>
+    <t>1e5a6686-6050-46fa-88fd-1c55588295f8</t>
+  </si>
+  <si>
+    <t>03afd8f8-cde4-4256-9fce-2f5e2978c622</t>
+  </si>
+  <si>
+    <t>c5734145-be7b-4493-b52d-f8b74ff890eb</t>
+  </si>
+  <si>
+    <t>7995ff37-9613-45b5-b03a-8320de1d3ebf</t>
+  </si>
+  <si>
+    <t>7cb284a5-b74c-45d3-8a4a-f0206e23fdf5</t>
+  </si>
+  <si>
+    <t>74f9ba2d-5805-4eec-9097-77e7aa07fa8c</t>
+  </si>
+  <si>
+    <t>21fc5f6f-78e2-40c2-9051-597d82972b28</t>
+  </si>
+  <si>
+    <t>d80db107-2572-483c-af0e-87f77eb9e051</t>
   </si>
 </sst>
 </file>
@@ -739,19 +739,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC0C0C0"/>
+        <fgColor rgb="FFFFC0CB"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFA8072"/>
+        <fgColor rgb="FFFF00FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF08080"/>
+        <fgColor rgb="FF8A2BE2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>

</xml_diff>